<commit_message>
📊 Update NAIC content history - 2025-09-04
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC590ED4-B0A8-4BB6-8B4D-386FAA840920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A94A58-0F5C-4D36-B488-71F18729910C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31005" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8004,85 +8004,85 @@
           <cell r="H246">
             <v>45899</v>
           </cell>
-          <cell r="I246" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J246" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K246" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L246" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I246">
+            <v>4.0599999999999997E-2</v>
+          </cell>
+          <cell r="J246">
+            <v>4.3799999999999999E-2</v>
+          </cell>
+          <cell r="K246">
+            <v>4.6300000000000001E-2</v>
+          </cell>
+          <cell r="L246">
+            <v>4.9000000000000002E-2</v>
           </cell>
         </row>
         <row r="247">
           <cell r="H247">
             <v>45900</v>
           </cell>
-          <cell r="I247" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J247" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K247" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L247" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I247">
+            <v>4.0599999999999997E-2</v>
+          </cell>
+          <cell r="J247">
+            <v>4.3799999999999999E-2</v>
+          </cell>
+          <cell r="K247">
+            <v>4.6300000000000001E-2</v>
+          </cell>
+          <cell r="L247">
+            <v>4.9000000000000002E-2</v>
           </cell>
         </row>
         <row r="248">
           <cell r="H248">
             <v>45901</v>
           </cell>
-          <cell r="I248" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J248" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K248" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L248" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I248">
+            <v>4.0599999999999997E-2</v>
+          </cell>
+          <cell r="J248">
+            <v>4.3799999999999999E-2</v>
+          </cell>
+          <cell r="K248">
+            <v>4.6300000000000001E-2</v>
+          </cell>
+          <cell r="L248">
+            <v>4.9000000000000002E-2</v>
           </cell>
         </row>
         <row r="249">
           <cell r="H249">
             <v>45902</v>
           </cell>
-          <cell r="I249" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J249" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K249" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L249" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I249">
+            <v>4.0599999999999997E-2</v>
+          </cell>
+          <cell r="J249">
+            <v>4.3799999999999999E-2</v>
+          </cell>
+          <cell r="K249">
+            <v>4.6300000000000001E-2</v>
+          </cell>
+          <cell r="L249">
+            <v>4.9000000000000002E-2</v>
           </cell>
         </row>
         <row r="250">
           <cell r="H250">
             <v>45903</v>
           </cell>
-          <cell r="I250" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J250" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K250" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L250" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I250">
+            <v>4.1200000000000001E-2</v>
+          </cell>
+          <cell r="J250">
+            <v>4.4499999999999998E-2</v>
+          </cell>
+          <cell r="K250">
+            <v>4.7100000000000003E-2</v>
+          </cell>
+          <cell r="L250">
+            <v>4.9700000000000001E-2</v>
           </cell>
         </row>
         <row r="251">
@@ -10422,7 +10422,7 @@
   <dimension ref="A1:E380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B244" sqref="B244"/>
     </sheetView>
   </sheetViews>
@@ -15777,21 +15777,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
       </c>
-      <c r="B245" s="17" t="str">
+      <c r="B245" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I246</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C245" s="48" t="str">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="C245" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J246</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D245" s="48" t="str">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="D245" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K246</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E245" s="5" t="str">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="E245" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L246</f>
-        <v xml:space="preserve"> </v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -15799,21 +15799,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
       </c>
-      <c r="B246" s="17" t="str">
+      <c r="B246" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I247</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C246" s="48" t="str">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="C246" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J247</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D246" s="48" t="str">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="D246" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K247</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E246" s="5" t="str">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="E246" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L247</f>
-        <v xml:space="preserve"> </v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -15821,21 +15821,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
       </c>
-      <c r="B247" s="17" t="str">
+      <c r="B247" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I248</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C247" s="48" t="str">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="C247" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J248</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D247" s="48" t="str">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="D247" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K248</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E247" s="5" t="str">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="E247" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L248</f>
-        <v xml:space="preserve"> </v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -15843,21 +15843,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
       </c>
-      <c r="B248" s="17" t="str">
+      <c r="B248" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I249</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C248" s="48" t="str">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="C248" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J249</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D248" s="48" t="str">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="D248" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K249</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E248" s="5" t="str">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="E248" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L249</f>
-        <v xml:space="preserve"> </v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -15865,21 +15865,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
       </c>
-      <c r="B249" s="17" t="str">
+      <c r="B249" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I250</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C249" s="48" t="str">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="C249" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J250</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D249" s="48" t="str">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="D249" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K250</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E249" s="5" t="str">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="E249" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L250</f>
-        <v xml:space="preserve"> </v>
+        <v>4.9700000000000001E-2</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -19390,182 +19390,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="str" cm="1">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="str">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-05
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A94A58-0F5C-4D36-B488-71F18729910C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F65E6D7-58F3-4897-A4BD-E31BBAC5AB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31005" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="10" windowWidth="18720" windowHeight="11660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -8089,17 +8089,17 @@
           <cell r="H251">
             <v>45904</v>
           </cell>
-          <cell r="I251" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J251" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K251" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L251" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I251">
+            <v>4.0800000000000003E-2</v>
+          </cell>
+          <cell r="J251">
+            <v>4.3900000000000002E-2</v>
+          </cell>
+          <cell r="K251">
+            <v>4.6399999999999997E-2</v>
+          </cell>
+          <cell r="L251">
+            <v>4.9000000000000002E-2</v>
           </cell>
         </row>
         <row r="252">
@@ -10423,19 +10423,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B244" sqref="B244"/>
+      <selection pane="bottomLeft" activeCell="F216" sqref="F216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10444,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10492,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10514,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10536,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10558,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10580,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10602,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10624,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10646,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10668,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10690,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10712,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10734,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10756,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10778,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10800,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10822,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10844,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10866,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10888,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10910,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10932,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10954,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10976,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10998,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11020,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11042,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11064,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11108,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11130,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11152,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11174,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11196,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11218,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11240,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11262,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11284,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11306,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11328,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11372,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11394,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11416,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11438,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11460,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11482,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11504,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11526,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11548,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11570,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11592,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11614,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11636,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11658,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11680,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11702,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11724,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11746,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11768,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11790,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11812,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11834,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11856,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11878,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11900,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11922,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11944,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11966,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11988,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12010,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12032,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12054,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12076,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12098,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12120,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12142,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12164,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12186,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12208,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12230,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12252,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12274,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12296,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12318,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12340,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12362,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12384,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12406,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12428,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12450,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12472,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12494,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12516,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12538,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12560,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12582,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12604,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12626,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12648,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12670,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12692,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12714,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12736,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12758,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12780,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12802,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12824,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12846,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12868,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12890,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12912,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12934,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12956,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12978,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +13000,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13022,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13044,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13066,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13088,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13110,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13132,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13154,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13176,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13198,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13220,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13242,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13264,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13286,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13308,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13330,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13352,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13374,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13396,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13418,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13440,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13462,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13484,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13506,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13528,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13550,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13572,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13594,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13616,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13638,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13660,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13682,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13704,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13726,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13748,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13770,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13792,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13814,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13836,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13858,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13880,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13902,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13924,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13946,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13968,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13990,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14012,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14034,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14056,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14078,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14100,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14122,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14144,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14166,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14188,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14210,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14232,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14254,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14276,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14298,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14320,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14364,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14386,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14408,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14430,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14452,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14474,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14496,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14518,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14540,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14562,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14584,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14606,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14628,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14650,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14672,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14716,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14738,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14760,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14782,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14804,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14826,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14848,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14870,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14892,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14914,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14936,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14958,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14980,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +15002,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15024,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15046,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15068,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15090,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15112,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15134,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15156,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15178,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15200,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15222,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15244,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15266,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15288,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15310,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15332,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15354,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15376,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15398,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15420,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15442,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15464,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15486,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15508,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15530,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15552,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15574,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15596,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15618,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15640,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15662,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15684,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15706,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15728,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15750,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15772,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15794,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15816,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15838,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15860,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,29 +15882,29 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
       </c>
-      <c r="B250" s="17" t="str">
+      <c r="B250" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I251</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C250" s="48" t="str">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="C250" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J251</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D250" s="48" t="str">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D250" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K251</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E250" s="5" t="str">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="E250" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L251</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15926,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15948,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15970,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,7 +15992,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16014,7 +16014,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,7 +16036,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16058,7 +16058,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16080,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16102,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16124,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,7 +16146,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -16168,7 +16168,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -16190,7 +16190,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -16212,7 +16212,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16234,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16256,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16278,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16300,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16322,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,7 +16344,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -16366,7 +16366,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16388,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16410,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16432,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,7 +16454,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -16476,7 +16476,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16498,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16520,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16542,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16586,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16630,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16674,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16718,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16740,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16762,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16784,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16828,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16850,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16872,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16894,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16916,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16938,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16982,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +17004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17026,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17048,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17070,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17092,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17158,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17180,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17202,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17246,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17290,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17334,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17378,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17400,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17422,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17466,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17488,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17510,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17554,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17598,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17620,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17686,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17708,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17730,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17774,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17796,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17818,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17862,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17906,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17950,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17972,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18016,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18038,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18082,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18126,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18170,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18192,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18214,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18236,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18258,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18346,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18390,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18412,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18500,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18522,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18573,13 +18573,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.28515625" customWidth="1"/>
+    <col min="2" max="5" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18588,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18604,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18613,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18652,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18674,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18696,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18718,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18740,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18764,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18778,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18819,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18843,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18867,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18891,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18899,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18907,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18917,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18927,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19041,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19049,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19069,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19085,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19105,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19125,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19145,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19165,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19174,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19254,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19289,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19324,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,15 +19381,15 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
@@ -19447,7 +19447,7 @@
       <c r="AT1" s="63"/>
       <c r="AU1" s="64"/>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
@@ -19505,7 +19505,7 @@
       <c r="AT2" s="66"/>
       <c r="AU2" s="67"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
@@ -19567,7 +19567,7 @@
       <c r="AT3" s="68"/>
       <c r="AU3" s="68"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20045,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20915,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21437,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22829,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +23003,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23873,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24047,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24221,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24569,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25294,7 +25294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-10
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE7D71A-1EE9-495B-ACBB-9D09CE92A17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21EB0D9-4676-41EE-AEB4-FCC3DACB8265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8174,17 +8174,17 @@
           <cell r="H256">
             <v>45909</v>
           </cell>
-          <cell r="I256" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J256" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K256" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L256" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I256">
+            <v>3.9300000000000002E-2</v>
+          </cell>
+          <cell r="J256">
+            <v>4.2200000000000001E-2</v>
+          </cell>
+          <cell r="K256">
+            <v>4.4499999999999998E-2</v>
+          </cell>
+          <cell r="L256">
+            <v>4.7E-2</v>
           </cell>
         </row>
         <row r="257">
@@ -10423,19 +10423,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E252" sqref="E252"/>
+      <selection pane="bottomLeft" activeCell="A255" sqref="A255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10444,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10492,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10514,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10536,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10558,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10580,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10602,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10624,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10646,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10668,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10690,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10712,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10734,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10756,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10778,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10800,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10822,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10844,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10866,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10888,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10910,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10932,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10954,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10976,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10998,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11020,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11042,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11064,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11108,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11130,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11152,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11174,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11196,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11218,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11240,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11262,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11284,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11306,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11328,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11372,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11394,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11416,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11438,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11460,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11482,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11504,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11526,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11548,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11570,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11592,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11614,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11636,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11658,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11680,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11702,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11724,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11746,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11768,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11790,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11812,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11834,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11856,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11878,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11900,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11922,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11944,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11966,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11988,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12010,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12032,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12054,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12076,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12098,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12120,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12142,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12164,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12186,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12208,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12230,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12252,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12274,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12296,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12318,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12340,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12362,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12384,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12406,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12428,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12450,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12472,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12494,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12516,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12538,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12560,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12582,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12604,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12626,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12648,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12670,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12692,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12714,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12736,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12758,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12780,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12802,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12824,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12846,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12868,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12890,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12912,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12934,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12956,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12978,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +13000,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13022,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13044,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13066,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13088,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13110,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13132,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13154,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13176,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13198,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13220,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13242,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13264,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13286,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13308,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13330,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13352,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13374,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13396,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13418,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13440,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13462,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13484,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13506,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13528,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13550,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13572,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13594,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13616,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13638,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13660,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13682,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13704,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13726,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13748,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13770,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13792,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13814,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13836,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13858,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13880,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13902,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13924,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13946,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13968,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13990,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14012,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14034,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14056,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14078,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14100,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14122,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14144,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14166,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14188,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14210,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14232,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14254,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14276,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14298,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14320,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14364,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14386,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14408,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14430,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14452,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14474,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14496,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14518,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14540,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14562,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14584,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14606,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14628,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14650,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14672,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14716,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14738,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14760,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14782,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14804,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14826,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14848,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14870,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14892,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14914,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14936,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14958,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14980,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +15002,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15024,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15046,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15068,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15090,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15112,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15134,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15156,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15178,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15200,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15222,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15244,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15266,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15288,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15310,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15332,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15354,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15376,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15398,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15420,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15442,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15464,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15486,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15508,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15530,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15552,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15574,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15596,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15618,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15640,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15662,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15684,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15706,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15728,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15750,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15772,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15794,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15816,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15838,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15860,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,7 +15882,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -15904,7 +15904,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15926,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15948,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15970,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,29 +15992,29 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
       </c>
-      <c r="B255" s="17" t="str">
+      <c r="B255" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I256</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C255" s="48" t="str">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="C255" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J256</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D255" s="48" t="str">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="D255" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K256</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E255" s="5" t="str">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="E255" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L256</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,7 +16036,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16058,7 +16058,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16080,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16102,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16124,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,7 +16146,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -16168,7 +16168,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -16190,7 +16190,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -16212,7 +16212,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16234,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16256,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16278,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16300,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16322,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,7 +16344,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -16366,7 +16366,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16388,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16410,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16432,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,7 +16454,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -16476,7 +16476,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16498,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16520,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16542,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16586,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16630,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16674,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16718,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16740,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16762,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16784,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16828,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16850,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16872,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16894,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16916,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16938,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16982,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +17004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17026,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17048,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17070,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17092,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17158,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17180,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17202,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17246,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17290,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17334,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17378,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17400,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17422,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17466,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17488,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17510,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17554,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17598,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17620,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17686,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17708,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17730,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17774,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17796,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17818,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17862,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17906,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17950,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17972,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18016,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18038,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18082,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18126,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18170,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18192,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18214,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18236,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18258,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18346,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18390,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18412,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18500,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18522,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18573,13 +18573,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.26953125" customWidth="1"/>
+    <col min="2" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18588,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18604,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18613,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18652,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18674,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18696,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18718,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18740,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18764,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18778,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18819,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18843,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18867,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18891,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18899,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18907,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18917,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18927,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19041,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19049,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19069,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19085,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19105,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19125,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19145,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19165,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19174,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19254,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19289,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19324,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,193 +19381,193 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="str">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20045,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20915,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21437,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22829,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +23003,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23873,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24047,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24221,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24569,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25294,7 +25294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-11
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21EB0D9-4676-41EE-AEB4-FCC3DACB8265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B7F855-F864-4FA3-921A-E2C3ACD55F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31980" yWindow="870" windowWidth="23385" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8191,17 +8191,17 @@
           <cell r="H257">
             <v>45910</v>
           </cell>
-          <cell r="I257" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J257" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K257" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L257" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I257">
+            <v>3.9699999999999999E-2</v>
+          </cell>
+          <cell r="J257">
+            <v>4.2599999999999999E-2</v>
+          </cell>
+          <cell r="K257">
+            <v>4.4900000000000002E-2</v>
+          </cell>
+          <cell r="L257">
+            <v>4.7300000000000002E-2</v>
           </cell>
         </row>
         <row r="258">
@@ -16019,21 +16019,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
       </c>
-      <c r="B256" s="17" t="str">
+      <c r="B256" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I257</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C256" s="48" t="str">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C256" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J257</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D256" s="48" t="str">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="D256" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K257</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E256" s="5" t="str">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="E256" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L257</f>
-        <v xml:space="preserve"> </v>
+        <v>4.7300000000000002E-2</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -19390,182 +19390,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="str" cm="1">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="str">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-12
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B7F855-F864-4FA3-921A-E2C3ACD55F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DBCCD1-49BD-4044-A29E-E6D62B956FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="870" windowWidth="23385" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -704,8 +704,8 @@
       <definedName name="Year_of_Valuation" refersTo="='History Tables'!$D$1"/>
     </definedNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="1">
           <cell r="D1">
@@ -713,10 +713,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7">
         <row r="6">
           <cell r="Q6">
@@ -955,8 +955,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
       <sheetData sheetId="10">
         <row r="6">
           <cell r="N6">
@@ -3812,11 +3812,6 @@
         </row>
       </sheetData>
       <sheetData sheetId="11">
-        <row r="1">
-          <cell r="D1" t="str">
-            <v>Sec. 3.C.4</v>
-          </cell>
-        </row>
         <row r="14">
           <cell r="D14">
             <v>4.4999999999999998E-2</v>
@@ -3898,10 +3893,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
       <sheetData sheetId="16">
         <row r="5">
           <cell r="H5">
@@ -8208,17 +8203,17 @@
           <cell r="H258">
             <v>45911</v>
           </cell>
-          <cell r="I258" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J258" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K258" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L258" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I258">
+            <v>3.9399999999999998E-2</v>
+          </cell>
+          <cell r="J258">
+            <v>4.2099999999999999E-2</v>
+          </cell>
+          <cell r="K258">
+            <v>4.4400000000000002E-2</v>
+          </cell>
+          <cell r="L258">
+            <v>4.6800000000000001E-2</v>
           </cell>
         </row>
         <row r="259">
@@ -10423,19 +10418,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A255" sqref="A255"/>
+      <selection pane="bottomLeft" activeCell="G245" sqref="G245"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10439,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10448,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10487,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10509,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10531,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10553,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10575,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10597,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10619,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10641,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10663,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10685,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10707,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10729,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10751,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10773,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10795,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10817,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10839,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10861,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10883,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10905,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10927,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10949,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10971,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10993,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11015,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11037,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11059,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11081,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11103,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11125,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11147,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11169,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11191,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11213,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11235,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11257,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11279,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11301,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11323,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11345,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11367,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11389,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11411,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11433,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11455,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11477,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11499,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11521,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11543,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11565,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11587,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11609,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11631,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11653,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11675,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11697,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11719,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11741,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11763,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11785,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11807,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11829,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11851,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11873,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11895,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11917,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11939,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11961,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11983,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12005,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12027,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12049,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12071,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12093,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12115,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12137,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12159,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12181,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12203,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12225,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12247,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12269,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12291,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12313,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12335,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12357,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12379,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12401,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12423,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12445,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12467,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12489,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12511,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12533,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12555,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12577,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12599,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12621,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12643,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12665,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12687,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12709,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12731,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12753,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12775,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12797,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12819,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12841,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12863,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12885,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12907,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12929,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12951,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12973,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +12995,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13017,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13039,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13061,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13083,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13105,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13127,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13149,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13171,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13193,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13215,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13237,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13259,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13281,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13303,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13325,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13347,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13369,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13391,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13413,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13435,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13457,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13479,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13501,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13523,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13545,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13567,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13589,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13611,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13633,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13655,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13677,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13699,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13721,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13743,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13765,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13787,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13809,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13831,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13853,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13875,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13897,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13919,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13941,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13963,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13985,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14007,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14029,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14051,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14073,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14095,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14117,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14139,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14161,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14183,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14205,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14227,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14249,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14271,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14293,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14315,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14337,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14359,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14381,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14403,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14425,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14447,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14469,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14491,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14513,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14535,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14557,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14579,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14601,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14623,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14645,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14667,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14689,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14711,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14733,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14755,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14777,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14799,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14821,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14843,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14865,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14887,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14909,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14931,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14953,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14975,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +14997,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15019,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15041,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15063,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15085,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15107,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15129,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15151,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15173,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15195,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15217,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15239,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15261,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15283,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15305,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15327,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15349,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15371,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15393,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15415,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15437,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15459,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15481,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15503,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15525,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15547,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15569,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15591,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15613,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15635,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15657,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15679,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15701,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15723,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15745,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15767,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15789,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15811,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15833,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15855,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,7 +15877,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -15904,7 +15899,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15921,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15943,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15965,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,7 +15987,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16014,7 +16009,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,29 +16031,29 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
       </c>
-      <c r="B257" s="17" t="str">
+      <c r="B257" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I258</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C257" s="48" t="str">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="C257" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J258</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D257" s="48" t="str">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="D257" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K258</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E257" s="5" t="str">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="E257" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L258</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.6800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,7 +16141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -16168,7 +16163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -16190,7 +16185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -16212,7 +16207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,7 +16339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -16366,7 +16361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,7 +16449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -16476,7 +16471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +16999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17659,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17681,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17703,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17725,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17747,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17769,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17791,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17813,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17835,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17857,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17879,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17901,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17923,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17945,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17967,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17989,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18011,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18033,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18055,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18077,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18099,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18121,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18143,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18165,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18187,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18209,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18231,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18253,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18275,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18297,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18319,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18341,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18363,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18385,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18407,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18429,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18451,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18473,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18495,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18517,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18573,13 +18568,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.28515625" customWidth="1"/>
+    <col min="2" max="5" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18583,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18599,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18608,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18647,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18669,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18691,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18713,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18735,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18750,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18759,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18773,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18814,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18838,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18862,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18886,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18894,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18902,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18912,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18922,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18940,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18962,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18984,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19006,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19028,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19036,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19044,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19054,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19064,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19080,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19100,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19120,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19140,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19160,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19169,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19180,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19191,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19214,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19249,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19284,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19319,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,193 +19376,193 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="str">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19866,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20040,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20214,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20388,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20562,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20736,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20910,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21084,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21258,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21432,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21606,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21780,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21954,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22128,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22302,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22476,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22650,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22824,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +22998,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23172,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23346,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23520,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23694,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23868,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24042,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24216,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24390,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24564,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24738,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24912,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25086,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25267,18 +25262,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25294,7 +25289,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-17
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5FDE1D-0228-4093-9F21-18E784733535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4A39C1-A2B3-4D12-93C1-E035EB372757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8293,17 +8293,17 @@
           <cell r="H263">
             <v>45916</v>
           </cell>
-          <cell r="I263" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J263" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K263" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L263" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I263">
+            <v>3.9E-2</v>
+          </cell>
+          <cell r="J263">
+            <v>4.1700000000000001E-2</v>
+          </cell>
+          <cell r="K263">
+            <v>4.3900000000000002E-2</v>
+          </cell>
+          <cell r="L263">
+            <v>4.6199999999999998E-2</v>
           </cell>
         </row>
         <row r="264">
@@ -10422,20 +10422,20 @@
   <dimension ref="A1:E380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E259" sqref="E259"/>
+      <pane ySplit="3" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A262" sqref="A262"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10444,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10492,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10514,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10536,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10558,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10580,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10602,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10624,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10646,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10668,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10690,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10712,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10734,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10756,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10778,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10800,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10822,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10844,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10866,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10888,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10910,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10932,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10954,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10976,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10998,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11020,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11042,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11064,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11108,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11130,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11152,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11174,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11196,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11218,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11240,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11262,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11284,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11306,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11328,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11372,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11394,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11416,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11438,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11460,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11482,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11504,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11526,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11548,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11570,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11592,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11614,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11636,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11658,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11680,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11702,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11724,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11746,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11768,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11790,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11812,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11834,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11856,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11878,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11900,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11922,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11944,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11966,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11988,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12010,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12032,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12054,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12076,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12098,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12120,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12142,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12164,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12186,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12208,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12230,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12252,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12274,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12296,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12318,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12340,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12362,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12384,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12406,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12428,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12450,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12472,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12494,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12516,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12538,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12560,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12582,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12604,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12626,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12648,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12670,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12692,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12714,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12736,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12758,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12780,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12802,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12824,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12846,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12868,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12890,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12912,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12934,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12956,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12978,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +13000,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13022,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13044,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13066,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13088,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13110,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13132,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13154,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13176,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13198,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13220,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13242,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13264,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13286,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13308,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13330,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13352,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13374,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13396,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13418,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13440,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13462,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13484,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13506,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13528,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13550,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13572,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13594,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13616,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13638,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13660,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13682,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13704,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13726,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13748,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13770,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13792,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13814,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13836,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13858,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13880,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13902,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13924,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13946,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13968,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13990,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14012,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14034,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14056,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14078,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14100,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14122,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14144,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14166,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14188,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14210,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14232,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14254,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14276,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14298,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14320,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14364,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14386,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14408,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14430,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14452,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14474,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14496,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14518,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14540,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14562,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14584,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14606,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14628,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14650,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14672,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14716,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14738,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14760,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14782,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14804,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14826,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14848,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14870,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14892,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14914,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14936,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14958,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14980,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +15002,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15024,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15046,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15068,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15090,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15112,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15134,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15156,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15178,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15200,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15222,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15244,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15266,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15288,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15310,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15332,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15354,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15376,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15398,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15420,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15442,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15464,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15486,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15508,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15530,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15552,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15574,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15596,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15618,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15640,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15662,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15684,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15706,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15728,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15750,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15772,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15794,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15816,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15838,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15860,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,7 +15882,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -15904,7 +15904,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15926,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15948,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15970,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,7 +15992,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16014,7 +16014,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,7 +16036,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16058,7 +16058,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16080,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16102,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16124,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,29 +16146,29 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
       </c>
-      <c r="B262" s="17" t="str">
+      <c r="B262" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I263</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C262" s="48" t="str">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C262" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J263</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D262" s="48" t="str">
+        <v>4.1700000000000001E-2</v>
+      </c>
+      <c r="D262" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K263</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E262" s="5" t="str">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="E262" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L263</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.6199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -16190,7 +16190,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -16212,7 +16212,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16234,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16256,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16278,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16300,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16322,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,7 +16344,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -16366,7 +16366,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16388,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16410,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16432,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,7 +16454,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -16476,7 +16476,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16498,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16520,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16542,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16586,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16630,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16674,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16718,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16740,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16762,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16784,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16828,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16850,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16872,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16894,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16916,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16938,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16982,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +17004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17026,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17048,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17070,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17092,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17158,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17180,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17202,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17246,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17290,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17334,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17378,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17400,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17422,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17466,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17488,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17510,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17554,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17598,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17620,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17686,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17708,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17730,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17774,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17796,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17818,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17862,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17906,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17950,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17972,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18016,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18038,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18082,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18126,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18170,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18192,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18214,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18236,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18258,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18346,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18390,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18412,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18500,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18522,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18573,13 +18573,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.26953125" customWidth="1"/>
+    <col min="2" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18588,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18604,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18613,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18652,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18674,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18696,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18718,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18740,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18764,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18778,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18819,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18843,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18867,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18891,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18899,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18907,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18917,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18927,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19041,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19049,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19069,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19085,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19105,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19125,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19145,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19165,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19174,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19254,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19289,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19324,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,193 +19381,193 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="str">
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20045,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20915,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21437,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22829,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +23003,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23873,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24047,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24221,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24569,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25294,7 +25294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-18
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4A39C1-A2B3-4D12-93C1-E035EB372757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD538D-D9DD-48C4-8D06-69BCC0F6F1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4188" yWindow="4188" windowWidth="22464" windowHeight="14136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -8310,17 +8310,17 @@
           <cell r="H264">
             <v>45917</v>
           </cell>
-          <cell r="I264" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J264" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K264" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L264" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I264">
+            <v>3.8800000000000001E-2</v>
+          </cell>
+          <cell r="J264">
+            <v>4.1599999999999998E-2</v>
+          </cell>
+          <cell r="K264">
+            <v>4.3799999999999999E-2</v>
+          </cell>
+          <cell r="L264">
+            <v>4.6199999999999998E-2</v>
           </cell>
         </row>
         <row r="265">
@@ -10426,16 +10426,16 @@
       <selection pane="bottomLeft" activeCell="A262" sqref="A262"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10444,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10492,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10514,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10536,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10558,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10580,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10602,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10624,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10646,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10668,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10690,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10712,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10734,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10756,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10778,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10800,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10822,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10844,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10866,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10888,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10910,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10932,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10954,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10976,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10998,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11020,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11042,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11064,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11108,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11130,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11152,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11174,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11196,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11218,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11240,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11262,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11284,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11306,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11328,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11372,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11394,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11416,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11438,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11460,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11482,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11504,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11526,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11548,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11570,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11592,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11614,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11636,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11658,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11680,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11702,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11724,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11746,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11768,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11790,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11812,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11834,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11856,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11878,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11900,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11922,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11944,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11966,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11988,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12010,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12032,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12054,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12076,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12098,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12120,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12142,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12164,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12186,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12208,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12230,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12252,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12274,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12296,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12318,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12340,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12362,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12384,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12406,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12428,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12450,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12472,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12494,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12516,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12538,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12560,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12582,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12604,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12626,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12648,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12670,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12692,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12714,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12736,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12758,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12780,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12802,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12824,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12846,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12868,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12890,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12912,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12934,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12956,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12978,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +13000,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13022,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13044,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13066,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13088,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13110,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13132,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13154,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13176,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13198,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13220,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13242,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13264,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13286,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13308,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13330,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13352,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13374,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13396,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13418,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13440,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13462,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13484,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13506,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13528,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13550,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13572,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13594,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13616,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13638,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13660,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13682,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13704,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13726,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13748,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13770,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13792,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13814,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13836,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13858,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13880,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13902,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13924,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13946,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13968,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13990,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14012,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14034,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14056,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14078,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14100,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14122,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14144,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14166,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14188,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14210,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14232,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14254,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14276,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14298,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14320,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14364,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14386,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14408,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14430,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14452,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14474,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14496,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14518,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14540,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14562,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14584,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14606,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14628,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14650,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14672,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14716,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14738,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14760,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14782,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14804,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14826,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14848,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14870,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14892,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14914,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14936,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14958,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14980,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +15002,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15024,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15046,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15068,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15090,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15112,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15134,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15156,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15178,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15200,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15222,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15244,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15266,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15288,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15310,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15332,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15354,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15376,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15398,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15420,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15442,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15464,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15486,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15508,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15530,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15552,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15574,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15596,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15618,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15640,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15662,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15684,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15706,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15728,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15750,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15772,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15794,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15816,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15838,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15860,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,7 +15882,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -15904,7 +15904,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15926,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15948,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15970,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,7 +15992,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16014,7 +16014,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,7 +16036,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16058,7 +16058,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16080,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16102,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16124,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,7 +16146,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -16168,29 +16168,29 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
       </c>
-      <c r="B263" s="17" t="str">
+      <c r="B263" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I264</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C263" s="48" t="str">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="C263" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J264</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D263" s="48" t="str">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="D263" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K264</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E263" s="5" t="str">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="E263" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L264</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.6199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -16212,7 +16212,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16234,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16256,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16278,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16300,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16322,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,7 +16344,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -16366,7 +16366,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16388,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16410,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16432,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,7 +16454,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -16476,7 +16476,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16498,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16520,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16542,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16586,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16630,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16674,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16718,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16740,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16762,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16784,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16828,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16850,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16872,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16894,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16916,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16938,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16982,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +17004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17026,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17048,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17070,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17092,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17158,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17180,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17202,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17246,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17290,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17334,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17378,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17400,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17422,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17466,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17488,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17510,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17554,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17598,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17620,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17686,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17708,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17730,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17774,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17796,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17818,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17862,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17906,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17950,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17972,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18016,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18038,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18082,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18126,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18170,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18192,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18214,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18236,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18258,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18346,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18390,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18412,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18500,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18522,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18573,13 +18573,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.28515625" customWidth="1"/>
+    <col min="2" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18588,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18604,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18613,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18652,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18674,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18696,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18718,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18740,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18764,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18778,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18819,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18843,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18867,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18891,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18899,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18907,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18917,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18927,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19041,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19049,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19069,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19085,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19105,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19125,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19145,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19165,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19174,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19254,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19289,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19324,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,193 +19381,193 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="str">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20045,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20915,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21437,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22829,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +23003,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23873,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24047,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24221,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24569,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25294,7 +25294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25315,7 +25315,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
+                <xdr:colOff>480060</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-19
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD538D-D9DD-48C4-8D06-69BCC0F6F1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D9C921-DA3B-4A44-B64E-153A920D833C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="4188" windowWidth="22464" windowHeight="14136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>482600</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -8327,17 +8327,17 @@
           <cell r="H265">
             <v>45918</v>
           </cell>
-          <cell r="I265" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J265" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K265" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L265" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I265">
+            <v>3.9199999999999999E-2</v>
+          </cell>
+          <cell r="J265">
+            <v>4.19E-2</v>
+          </cell>
+          <cell r="K265">
+            <v>4.41E-2</v>
+          </cell>
+          <cell r="L265">
+            <v>4.65E-2</v>
           </cell>
         </row>
         <row r="266">
@@ -10423,19 +10423,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A262" sqref="A262"/>
+      <selection pane="bottomLeft" activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10444,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10492,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10514,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10536,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10558,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10580,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10602,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10624,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10646,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10668,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10690,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10712,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10734,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10756,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10778,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10800,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10822,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10844,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10866,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10888,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10910,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10932,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10954,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10976,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10998,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11020,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11042,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11064,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11108,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11130,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11152,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11174,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11196,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11218,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11240,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11262,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11284,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11306,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11328,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11372,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11394,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11416,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11438,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11460,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11482,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11504,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11526,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11548,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11570,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11592,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11614,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11636,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11658,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11680,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11702,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11724,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11746,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11768,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11790,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11812,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11834,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11856,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11878,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11900,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11922,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11944,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11966,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11988,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12010,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12032,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12054,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12076,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12098,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12120,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12142,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12164,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12186,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12208,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12230,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12252,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12274,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12296,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12318,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12340,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12362,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12384,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12406,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12428,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12450,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12472,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12494,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12516,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12538,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12560,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12582,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12604,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12626,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12648,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12670,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12692,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12714,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12736,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12758,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12780,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12802,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12824,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12846,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12868,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12890,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12912,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12934,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12956,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12978,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +13000,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13022,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13044,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13066,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13088,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13110,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13132,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13154,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13176,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13198,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13220,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13242,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13264,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13286,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13308,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13330,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13352,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13374,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13396,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13418,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13440,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13462,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13484,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13506,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13528,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13550,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13572,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13594,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13616,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13638,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13660,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13682,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13704,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13726,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13748,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13770,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13792,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13814,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13836,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13858,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13880,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13902,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13924,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13946,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13968,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13990,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14012,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14034,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14056,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14078,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14100,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14122,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14144,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14166,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14188,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14210,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14232,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14254,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14276,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14298,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14320,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14364,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14386,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14408,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14430,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14452,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14474,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14496,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14518,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14540,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14562,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14584,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14606,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14628,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14650,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14672,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14716,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14738,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14760,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14782,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14804,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14826,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14848,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14870,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14892,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14914,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14936,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14958,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14980,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +15002,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15024,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15046,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15068,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15090,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15112,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15134,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15156,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15178,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15200,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15222,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15244,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15266,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15288,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15310,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15332,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15354,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15376,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15398,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15420,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15442,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15464,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15486,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15508,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15530,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15552,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15574,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15596,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15618,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15640,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15662,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15684,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15706,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15728,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15750,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15772,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15794,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15816,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15838,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15860,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,7 +15882,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -15904,7 +15904,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15926,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15948,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15970,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,7 +15992,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16014,7 +16014,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,7 +16036,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16058,7 +16058,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16080,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16102,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16124,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,7 +16146,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -16168,7 +16168,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -16190,29 +16190,29 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
       </c>
-      <c r="B264" s="17" t="str">
+      <c r="B264" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I265</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C264" s="48" t="str">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="C264" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J265</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D264" s="48" t="str">
+        <v>4.19E-2</v>
+      </c>
+      <c r="D264" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K265</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E264" s="5" t="str">
+        <v>4.41E-2</v>
+      </c>
+      <c r="E264" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L265</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.65E-2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16234,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16256,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16278,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16300,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16322,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,7 +16344,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -16366,7 +16366,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16388,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16410,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16432,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,7 +16454,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -16476,7 +16476,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16498,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16520,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16542,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16586,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16630,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16674,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16718,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16740,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16762,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16784,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16828,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16850,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16872,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16894,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16916,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16938,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16982,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +17004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17026,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17048,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17070,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17092,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17158,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17180,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17202,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17246,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17290,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17334,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17378,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17400,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17422,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17466,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17488,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17510,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17554,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17598,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17620,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17686,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17708,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17730,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17774,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17796,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17818,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17862,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17906,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17950,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17972,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18016,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18038,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18082,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18126,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18170,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18192,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18214,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18236,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18258,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18346,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18390,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18412,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18500,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18522,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18570,16 +18570,16 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.33203125" customWidth="1"/>
+    <col min="2" max="5" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18588,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18604,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18613,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18652,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18674,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18696,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18718,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18740,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18764,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18778,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18819,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18843,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18867,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18891,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18899,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18907,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18917,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18927,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19041,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19049,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19069,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19085,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19105,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19125,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19145,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19165,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19174,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19254,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19289,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19324,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,15 +19381,15 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
@@ -19447,7 +19447,7 @@
       <c r="AT1" s="67"/>
       <c r="AU1" s="68"/>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
@@ -19505,7 +19505,7 @@
       <c r="AT2" s="63"/>
       <c r="AU2" s="64"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
@@ -19567,7 +19567,7 @@
       <c r="AT3" s="65"/>
       <c r="AU3" s="65"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20045,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20915,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21437,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22829,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +23003,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23873,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24047,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24221,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24569,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25294,7 +25294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25315,7 +25315,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>480060</xdr:colOff>
+                <xdr:colOff>482600</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-26
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E22852-047E-40CC-B007-BBFC3812EF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13F8D7-D0E3-4DE2-BA85-08A6B89143AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="1590" windowWidth="22395" windowHeight="13125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
+          <xdr:colOff>488950</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -8446,17 +8446,17 @@
           <cell r="H272">
             <v>45925</v>
           </cell>
-          <cell r="I272" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J272" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K272" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L272" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I272">
+            <v>3.9800000000000002E-2</v>
+          </cell>
+          <cell r="J272">
+            <v>4.2599999999999999E-2</v>
+          </cell>
+          <cell r="K272">
+            <v>4.4900000000000002E-2</v>
+          </cell>
+          <cell r="L272">
+            <v>4.7300000000000002E-2</v>
           </cell>
         </row>
         <row r="273">
@@ -10426,16 +10426,16 @@
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10444,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10492,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10514,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10536,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10558,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10580,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10602,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10624,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10646,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10668,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10690,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10712,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10734,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10756,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10778,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10800,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10822,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10844,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10866,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10888,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10910,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10932,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10954,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10976,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10998,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11020,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11042,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11064,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11108,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11130,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11152,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11174,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11196,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11218,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11240,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11262,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11284,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11306,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11328,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11372,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11394,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11416,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11438,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11460,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11482,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11504,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11526,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11548,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11570,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11592,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11614,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11636,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11658,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11680,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11702,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11724,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11746,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11768,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11790,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11812,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11834,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11856,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11878,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11900,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11922,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11944,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11966,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11988,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12010,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12032,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12054,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12076,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12098,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12120,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12142,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12164,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12186,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12208,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12230,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12252,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12274,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12296,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12318,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12340,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12362,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12384,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12406,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12428,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12450,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12472,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12494,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12516,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12538,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12560,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12582,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12604,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12626,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12648,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12670,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12692,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12714,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12736,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12758,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12780,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12802,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12824,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12846,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12868,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12890,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12912,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12934,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12956,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12978,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +13000,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13022,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13044,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13066,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13088,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13110,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13132,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13154,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13176,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13198,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13220,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13242,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13264,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13286,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13308,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13330,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13352,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13374,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13396,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13418,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13440,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13462,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13484,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13506,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13528,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13550,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13572,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13594,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13616,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13638,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13660,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13682,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13704,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13726,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13748,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13770,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13792,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13814,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13836,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13858,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13880,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13902,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13924,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13946,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13968,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13990,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14012,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14034,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14056,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14078,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14100,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14122,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14144,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14166,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14188,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14210,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14232,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14254,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14276,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14298,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14320,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14364,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14386,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14408,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14430,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14452,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14474,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14496,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14518,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14540,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14562,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14584,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14606,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14628,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14650,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14672,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14716,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14738,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14760,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14782,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14804,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14826,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14848,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14870,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14892,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14914,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14936,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14958,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14980,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +15002,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15024,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15046,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15068,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15090,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15112,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15134,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15156,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15178,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15200,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15222,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15244,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15266,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15288,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15310,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15332,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15354,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15376,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15398,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15420,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15442,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15464,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15486,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15508,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15530,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15552,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15574,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15596,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15618,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15640,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15662,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15684,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15706,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15728,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15750,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15772,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15794,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15816,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15838,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15860,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,7 +15882,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -15904,7 +15904,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15926,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15948,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15970,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,7 +15992,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16014,7 +16014,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,7 +16036,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16058,7 +16058,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16080,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16102,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16124,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,7 +16146,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -16168,7 +16168,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -16190,7 +16190,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -16212,7 +16212,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16234,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16256,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16278,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16300,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16322,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,29 +16344,29 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
       </c>
-      <c r="B271" s="17" t="str">
+      <c r="B271" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I272</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C271" s="48" t="str">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="C271" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J272</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D271" s="48" t="str">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="D271" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K272</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E271" s="5" t="str">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="E271" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L272</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.7300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16388,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16410,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16432,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,7 +16454,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -16476,7 +16476,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16498,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16520,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16542,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16586,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16630,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16674,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16718,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16740,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16762,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16784,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16828,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16850,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16872,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16894,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16916,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16938,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16982,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +17004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17026,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17048,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17070,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17092,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17158,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17180,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17202,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17246,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17290,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17334,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17378,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17400,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17422,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17466,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17488,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17510,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17554,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17598,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17620,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17686,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17708,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17730,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17774,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17796,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17818,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17862,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17906,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17950,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17972,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18016,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18038,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18082,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18126,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18170,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18192,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18214,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18236,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18258,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18346,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18390,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18412,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18500,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18522,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18573,13 +18573,13 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18588,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18604,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18613,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18652,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18674,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18696,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18718,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18740,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18764,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18778,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18819,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18843,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18867,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18891,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18899,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18907,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18917,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18927,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19041,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19049,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19069,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19085,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19105,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19125,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19145,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19165,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19174,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19254,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19289,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19324,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,193 +19381,193 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="str">
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20045,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20915,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21437,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22829,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +23003,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23873,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24047,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24221,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24569,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25294,7 +25294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25315,7 +25315,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
+                <xdr:colOff>488950</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-09-30
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13F8D7-D0E3-4DE2-BA85-08A6B89143AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84164D06-BB2F-4551-BB51-BA067FB83167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8463,68 +8463,68 @@
           <cell r="H273">
             <v>45926</v>
           </cell>
-          <cell r="I273" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J273" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K273" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L273" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I273">
+            <v>4.0300000000000002E-2</v>
+          </cell>
+          <cell r="J273">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K273">
+            <v>4.5199999999999997E-2</v>
+          </cell>
+          <cell r="L273">
+            <v>4.7600000000000003E-2</v>
           </cell>
         </row>
         <row r="274">
           <cell r="H274">
             <v>45927</v>
           </cell>
-          <cell r="I274" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J274" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K274" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L274" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I274">
+            <v>4.02E-2</v>
+          </cell>
+          <cell r="J274">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K274">
+            <v>4.5199999999999997E-2</v>
+          </cell>
+          <cell r="L274">
+            <v>4.7500000000000001E-2</v>
           </cell>
         </row>
         <row r="275">
           <cell r="H275">
             <v>45928</v>
           </cell>
-          <cell r="I275" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J275" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K275" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L275" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I275">
+            <v>4.02E-2</v>
+          </cell>
+          <cell r="J275">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K275">
+            <v>4.5199999999999997E-2</v>
+          </cell>
+          <cell r="L275">
+            <v>4.7500000000000001E-2</v>
           </cell>
         </row>
         <row r="276">
           <cell r="H276">
             <v>45929</v>
           </cell>
-          <cell r="I276" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J276" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K276" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L276" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I276">
+            <v>4.02E-2</v>
+          </cell>
+          <cell r="J276">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K276">
+            <v>4.5199999999999997E-2</v>
+          </cell>
+          <cell r="L276">
+            <v>4.7500000000000001E-2</v>
           </cell>
         </row>
         <row r="277">
@@ -10423,7 +10423,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E273" sqref="E273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16371,21 +16371,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
       </c>
-      <c r="B272" s="17" t="str">
+      <c r="B272" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I273</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C272" s="48" t="str">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="C272" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J273</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D272" s="48" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D272" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K273</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E272" s="5" t="str">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="E272" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L273</f>
-        <v xml:space="preserve"> </v>
+        <v>4.7600000000000003E-2</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.35">
@@ -16393,21 +16393,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
       </c>
-      <c r="B273" s="17" t="str">
+      <c r="B273" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I274</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C273" s="48" t="str">
+        <v>4.02E-2</v>
+      </c>
+      <c r="C273" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J274</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D273" s="48" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D273" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K274</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E273" s="5" t="str">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="E273" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L274</f>
-        <v xml:space="preserve"> </v>
+        <v>4.7500000000000001E-2</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.35">
@@ -16415,21 +16415,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
       </c>
-      <c r="B274" s="17" t="str">
+      <c r="B274" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I275</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C274" s="48" t="str">
+        <v>4.02E-2</v>
+      </c>
+      <c r="C274" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J275</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D274" s="48" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D274" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K275</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E274" s="5" t="str">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="E274" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L275</f>
-        <v xml:space="preserve"> </v>
+        <v>4.7500000000000001E-2</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.35">
@@ -16437,21 +16437,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
       </c>
-      <c r="B275" s="17" t="str">
+      <c r="B275" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I276</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C275" s="48" t="str">
+        <v>4.02E-2</v>
+      </c>
+      <c r="C275" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J276</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D275" s="48" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D275" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K276</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E275" s="5" t="str">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="E275" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L276</f>
-        <v xml:space="preserve"> </v>
+        <v>4.7500000000000001E-2</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.35">
@@ -19390,182 +19390,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="str" cm="1">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="str">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-01
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84164D06-BB2F-4551-BB51-BA067FB83167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EB6ACE-5DDA-437C-B69C-B622136142F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>488950</xdr:colOff>
+          <xdr:colOff>485775</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -8531,17 +8531,17 @@
           <cell r="H277">
             <v>45930</v>
           </cell>
-          <cell r="I277" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J277" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K277" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L277" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I277">
+            <v>3.9899999999999998E-2</v>
+          </cell>
+          <cell r="J277">
+            <v>4.2599999999999999E-2</v>
+          </cell>
+          <cell r="K277">
+            <v>4.4699999999999997E-2</v>
+          </cell>
+          <cell r="L277">
+            <v>4.7E-2</v>
           </cell>
         </row>
         <row r="278">
@@ -10423,19 +10423,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E273" sqref="E273"/>
+      <selection pane="bottomLeft" activeCell="B276" sqref="B276"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -10444,7 +10444,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -10492,7 +10492,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -10514,7 +10514,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -10536,7 +10536,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -10558,7 +10558,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -10580,7 +10580,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -10602,7 +10602,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -10624,7 +10624,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -10646,7 +10646,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -10668,7 +10668,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -10690,7 +10690,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -10712,7 +10712,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -10734,7 +10734,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -10756,7 +10756,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -10778,7 +10778,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -10800,7 +10800,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -10822,7 +10822,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -10844,7 +10844,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -10866,7 +10866,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -10888,7 +10888,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -10910,7 +10910,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -10932,7 +10932,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -10954,7 +10954,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -10976,7 +10976,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -10998,7 +10998,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11020,7 +11020,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11042,7 +11042,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11064,7 +11064,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -11086,7 +11086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -11108,7 +11108,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -11130,7 +11130,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -11152,7 +11152,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -11174,7 +11174,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -11196,7 +11196,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -11218,7 +11218,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -11240,7 +11240,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -11262,7 +11262,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -11284,7 +11284,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -11306,7 +11306,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -11328,7 +11328,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -11350,7 +11350,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -11372,7 +11372,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -11394,7 +11394,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -11416,7 +11416,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -11438,7 +11438,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -11460,7 +11460,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -11482,7 +11482,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -11504,7 +11504,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -11526,7 +11526,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -11548,7 +11548,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -11570,7 +11570,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -11592,7 +11592,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -11614,7 +11614,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -11636,7 +11636,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -11658,7 +11658,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -11680,7 +11680,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -11702,7 +11702,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -11724,7 +11724,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -11746,7 +11746,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -11768,7 +11768,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -11790,7 +11790,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -11812,7 +11812,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -11834,7 +11834,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -11856,7 +11856,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -11878,7 +11878,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -11900,7 +11900,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -11922,7 +11922,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -11944,7 +11944,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -11966,7 +11966,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -11988,7 +11988,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12010,7 +12010,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12032,7 +12032,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12054,7 +12054,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -12076,7 +12076,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -12098,7 +12098,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -12120,7 +12120,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -12142,7 +12142,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -12164,7 +12164,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -12186,7 +12186,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -12208,7 +12208,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -12230,7 +12230,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -12252,7 +12252,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -12274,7 +12274,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -12296,7 +12296,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -12318,7 +12318,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -12340,7 +12340,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -12362,7 +12362,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -12384,7 +12384,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -12406,7 +12406,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -12428,7 +12428,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -12450,7 +12450,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -12472,7 +12472,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -12494,7 +12494,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -12516,7 +12516,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -12538,7 +12538,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -12560,7 +12560,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -12582,7 +12582,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -12604,7 +12604,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -12626,7 +12626,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -12648,7 +12648,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -12670,7 +12670,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -12692,7 +12692,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -12714,7 +12714,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -12736,7 +12736,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -12758,7 +12758,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -12780,7 +12780,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -12802,7 +12802,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -12824,7 +12824,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -12846,7 +12846,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -12868,7 +12868,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -12890,7 +12890,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -12912,7 +12912,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -12934,7 +12934,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -12956,7 +12956,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -12978,7 +12978,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13000,7 +13000,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13022,7 +13022,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13044,7 +13044,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13066,7 +13066,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -13088,7 +13088,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -13110,7 +13110,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -13132,7 +13132,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -13154,7 +13154,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -13176,7 +13176,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -13198,7 +13198,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -13220,7 +13220,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -13242,7 +13242,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -13264,7 +13264,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -13286,7 +13286,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -13308,7 +13308,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -13330,7 +13330,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -13352,7 +13352,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -13374,7 +13374,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -13396,7 +13396,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -13418,7 +13418,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -13440,7 +13440,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -13462,7 +13462,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -13484,7 +13484,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -13506,7 +13506,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -13528,7 +13528,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -13550,7 +13550,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -13572,7 +13572,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -13594,7 +13594,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -13616,7 +13616,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -13638,7 +13638,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -13660,7 +13660,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -13682,7 +13682,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -13704,7 +13704,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -13726,7 +13726,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -13748,7 +13748,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -13770,7 +13770,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -13792,7 +13792,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -13814,7 +13814,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -13836,7 +13836,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -13858,7 +13858,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -13880,7 +13880,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -13902,7 +13902,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -13924,7 +13924,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -13946,7 +13946,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -13968,7 +13968,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -13990,7 +13990,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14012,7 +14012,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14034,7 +14034,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14056,7 +14056,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -14078,7 +14078,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -14100,7 +14100,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -14122,7 +14122,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -14144,7 +14144,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -14166,7 +14166,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -14188,7 +14188,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -14210,7 +14210,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -14232,7 +14232,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -14254,7 +14254,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -14276,7 +14276,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -14298,7 +14298,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -14320,7 +14320,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -14342,7 +14342,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -14364,7 +14364,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -14386,7 +14386,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -14408,7 +14408,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -14430,7 +14430,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -14452,7 +14452,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -14474,7 +14474,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -14496,7 +14496,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -14518,7 +14518,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -14540,7 +14540,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -14562,7 +14562,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -14584,7 +14584,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -14606,7 +14606,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -14628,7 +14628,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -14650,7 +14650,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -14672,7 +14672,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -14694,7 +14694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -14716,7 +14716,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -14738,7 +14738,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -14760,7 +14760,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -14782,7 +14782,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -14804,7 +14804,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -14826,7 +14826,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -14848,7 +14848,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -14870,7 +14870,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -14892,7 +14892,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -14914,7 +14914,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -14936,7 +14936,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -14958,7 +14958,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -14980,7 +14980,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15002,7 +15002,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15024,7 +15024,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15046,7 +15046,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15068,7 +15068,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -15090,7 +15090,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -15112,7 +15112,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -15134,7 +15134,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -15156,7 +15156,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -15178,7 +15178,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -15200,7 +15200,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -15222,7 +15222,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -15244,7 +15244,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -15266,7 +15266,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -15288,7 +15288,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -15310,7 +15310,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -15332,7 +15332,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -15354,7 +15354,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -15376,7 +15376,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -15398,7 +15398,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -15420,7 +15420,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -15442,7 +15442,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -15464,7 +15464,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -15486,7 +15486,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -15508,7 +15508,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -15530,7 +15530,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -15552,7 +15552,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -15574,7 +15574,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -15596,7 +15596,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -15618,7 +15618,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -15640,7 +15640,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -15662,7 +15662,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -15684,7 +15684,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -15706,7 +15706,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -15728,7 +15728,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -15750,7 +15750,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -15772,7 +15772,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -15794,7 +15794,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -15816,7 +15816,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -15838,7 +15838,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -15860,7 +15860,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -15882,7 +15882,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -15904,7 +15904,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -15926,7 +15926,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -15948,7 +15948,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -15970,7 +15970,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -15992,7 +15992,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16014,7 +16014,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16036,7 +16036,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16058,7 +16058,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -16080,7 +16080,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -16102,7 +16102,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -16124,7 +16124,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -16146,7 +16146,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -16168,7 +16168,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -16190,7 +16190,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -16212,7 +16212,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -16234,7 +16234,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -16256,7 +16256,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -16278,7 +16278,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -16300,7 +16300,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -16322,7 +16322,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -16344,7 +16344,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -16366,7 +16366,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -16388,7 +16388,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -16410,7 +16410,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -16432,7 +16432,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -16454,29 +16454,29 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
       </c>
-      <c r="B276" s="17" t="str">
+      <c r="B276" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I277</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C276" s="48" t="str">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="C276" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J277</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D276" s="48" t="str">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="D276" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K277</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E276" s="5" t="str">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="E276" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L277</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -16498,7 +16498,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -16520,7 +16520,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -16542,7 +16542,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -16564,7 +16564,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -16586,7 +16586,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -16608,7 +16608,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -16630,7 +16630,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -16652,7 +16652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -16674,7 +16674,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -16696,7 +16696,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -16718,7 +16718,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -16740,7 +16740,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -16762,7 +16762,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -16784,7 +16784,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -16806,7 +16806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -16828,7 +16828,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -16850,7 +16850,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -16872,7 +16872,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -16894,7 +16894,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -16916,7 +16916,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -16938,7 +16938,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -16960,7 +16960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -16982,7 +16982,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17004,7 +17004,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17026,7 +17026,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17048,7 +17048,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -17070,7 +17070,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -17092,7 +17092,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -17114,7 +17114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -17136,7 +17136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -17158,7 +17158,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -17180,7 +17180,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -17202,7 +17202,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -17224,7 +17224,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -17246,7 +17246,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -17268,7 +17268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -17290,7 +17290,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -17312,7 +17312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -17334,7 +17334,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -17356,7 +17356,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -17378,7 +17378,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -17400,7 +17400,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -17422,7 +17422,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -17444,7 +17444,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -17466,7 +17466,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -17488,7 +17488,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -17510,7 +17510,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -17532,7 +17532,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -17554,7 +17554,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -17576,7 +17576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -17598,7 +17598,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -17620,7 +17620,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -17642,7 +17642,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -17664,7 +17664,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -17686,7 +17686,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -17708,7 +17708,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -17730,7 +17730,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -17752,7 +17752,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -17774,7 +17774,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -17796,7 +17796,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -17818,7 +17818,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -17840,7 +17840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -17862,7 +17862,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -17884,7 +17884,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -17906,7 +17906,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -17928,7 +17928,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -17950,7 +17950,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -17972,7 +17972,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -17994,7 +17994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18016,7 +18016,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18038,7 +18038,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18060,7 +18060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -18082,7 +18082,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -18104,7 +18104,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -18126,7 +18126,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -18148,7 +18148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -18170,7 +18170,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -18192,7 +18192,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -18214,7 +18214,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -18236,7 +18236,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -18258,7 +18258,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -18280,7 +18280,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -18302,7 +18302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -18324,7 +18324,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -18346,7 +18346,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -18368,7 +18368,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -18390,7 +18390,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -18412,7 +18412,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -18434,7 +18434,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -18456,7 +18456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -18478,7 +18478,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -18500,7 +18500,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -18522,37 +18522,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -18573,13 +18573,13 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -18588,14 +18588,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -18604,7 +18604,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -18613,7 +18613,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -18652,7 +18652,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -18674,7 +18674,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -18696,7 +18696,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -18718,7 +18718,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -18740,13 +18740,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -18755,7 +18755,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -18764,12 +18764,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -18778,7 +18778,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -18795,7 +18795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -18819,7 +18819,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -18843,7 +18843,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -18867,7 +18867,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -18891,7 +18891,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -18899,7 +18899,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -18907,7 +18907,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -18917,7 +18917,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -18927,7 +18927,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19041,7 +19041,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19049,7 +19049,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19059,7 +19059,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19069,7 +19069,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -19085,7 +19085,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -19105,7 +19105,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -19125,7 +19125,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -19145,7 +19145,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -19165,7 +19165,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -19174,7 +19174,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -19254,7 +19254,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -19289,7 +19289,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -19324,7 +19324,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -19381,193 +19381,193 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="str">
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -19871,7 +19871,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20045,7 +20045,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -20915,7 +20915,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -21437,7 +21437,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -21611,7 +21611,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -21785,7 +21785,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -21959,7 +21959,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -22307,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -22829,7 +22829,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23003,7 +23003,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -23177,7 +23177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -23351,7 +23351,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -23873,7 +23873,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24047,7 +24047,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -24221,7 +24221,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -24395,7 +24395,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -24569,7 +24569,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -24917,7 +24917,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -25267,18 +25267,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25294,7 +25294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25315,7 +25315,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>488950</xdr:colOff>
+                <xdr:colOff>485775</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-03
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69C1538-F965-4329-80A5-387A04BBFD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D3C53B-6634-4FF7-9AFF-6D401008C44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
+          <xdr:colOff>488950</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -9495,17 +9495,17 @@
           <cell r="H279">
             <v>45932</v>
           </cell>
-          <cell r="I279" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J279" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K279" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L279" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I279">
+            <v>3.9199999999999999E-2</v>
+          </cell>
+          <cell r="J279">
+            <v>4.2200000000000001E-2</v>
+          </cell>
+          <cell r="K279">
+            <v>4.4600000000000001E-2</v>
+          </cell>
+          <cell r="L279">
+            <v>4.7100000000000003E-2</v>
           </cell>
         </row>
         <row r="280">
@@ -11351,21 +11351,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E380"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B277" sqref="B277"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -11374,7 +11374,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -11383,7 +11383,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -11422,7 +11422,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -11444,7 +11444,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -11466,7 +11466,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -11488,7 +11488,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -11510,7 +11510,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -11532,7 +11532,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -11554,7 +11554,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -11576,7 +11576,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -11598,7 +11598,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -11620,7 +11620,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -11642,7 +11642,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -11664,7 +11664,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -11686,7 +11686,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -11708,7 +11708,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -11730,7 +11730,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -11752,7 +11752,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -11774,7 +11774,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -11796,7 +11796,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -11818,7 +11818,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -11840,7 +11840,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -11862,7 +11862,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -11884,7 +11884,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -11906,7 +11906,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -11928,7 +11928,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11950,7 +11950,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11972,7 +11972,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11994,7 +11994,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -12016,7 +12016,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -12038,7 +12038,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -12060,7 +12060,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -12082,7 +12082,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -12104,7 +12104,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -12126,7 +12126,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -12148,7 +12148,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -12170,7 +12170,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -12192,7 +12192,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -12214,7 +12214,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -12236,7 +12236,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -12258,7 +12258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -12280,7 +12280,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -12302,7 +12302,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -12324,7 +12324,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -12346,7 +12346,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -12368,7 +12368,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -12390,7 +12390,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -12412,7 +12412,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -12434,7 +12434,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -12456,7 +12456,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -12478,7 +12478,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -12500,7 +12500,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -12522,7 +12522,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -12544,7 +12544,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -12566,7 +12566,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -12588,7 +12588,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -12610,7 +12610,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -12632,7 +12632,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -12654,7 +12654,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -12676,7 +12676,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -12698,7 +12698,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -12720,7 +12720,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -12742,7 +12742,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -12764,7 +12764,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -12786,7 +12786,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -12808,7 +12808,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -12830,7 +12830,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -12852,7 +12852,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -12874,7 +12874,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -12896,7 +12896,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -12918,7 +12918,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12940,7 +12940,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12962,7 +12962,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12984,7 +12984,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -13006,7 +13006,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -13028,7 +13028,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -13050,7 +13050,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -13072,7 +13072,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -13094,7 +13094,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -13116,7 +13116,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -13138,7 +13138,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -13160,7 +13160,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -13182,7 +13182,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -13204,7 +13204,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -13226,7 +13226,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -13248,7 +13248,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -13270,7 +13270,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -13292,7 +13292,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -13314,7 +13314,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -13336,7 +13336,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -13358,7 +13358,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -13380,7 +13380,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -13402,7 +13402,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -13424,7 +13424,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -13446,7 +13446,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -13468,7 +13468,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -13490,7 +13490,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -13512,7 +13512,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -13534,7 +13534,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -13556,7 +13556,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -13578,7 +13578,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -13600,7 +13600,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -13622,7 +13622,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -13644,7 +13644,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -13666,7 +13666,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -13688,7 +13688,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -13710,7 +13710,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -13732,7 +13732,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -13754,7 +13754,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -13776,7 +13776,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -13798,7 +13798,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -13820,7 +13820,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -13842,7 +13842,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -13864,7 +13864,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -13886,7 +13886,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -13908,7 +13908,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13930,7 +13930,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13952,7 +13952,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13974,7 +13974,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13996,7 +13996,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -14018,7 +14018,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -14040,7 +14040,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -14062,7 +14062,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -14084,7 +14084,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -14106,7 +14106,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -14128,7 +14128,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -14150,7 +14150,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -14172,7 +14172,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -14194,7 +14194,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -14216,7 +14216,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -14238,7 +14238,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -14260,7 +14260,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -14282,7 +14282,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -14304,7 +14304,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -14326,7 +14326,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -14348,7 +14348,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -14370,7 +14370,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -14392,7 +14392,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -14414,7 +14414,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -14436,7 +14436,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -14458,7 +14458,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -14480,7 +14480,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -14502,7 +14502,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -14524,7 +14524,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -14546,7 +14546,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -14568,7 +14568,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -14590,7 +14590,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -14612,7 +14612,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -14634,7 +14634,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -14656,7 +14656,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -14678,7 +14678,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -14700,7 +14700,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -14722,7 +14722,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -14744,7 +14744,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -14766,7 +14766,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -14788,7 +14788,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -14810,7 +14810,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -14832,7 +14832,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -14854,7 +14854,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -14876,7 +14876,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -14898,7 +14898,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -14920,7 +14920,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14942,7 +14942,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14964,7 +14964,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14986,7 +14986,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -15008,7 +15008,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -15030,7 +15030,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -15052,7 +15052,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -15074,7 +15074,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -15096,7 +15096,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -15118,7 +15118,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -15140,7 +15140,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -15162,7 +15162,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -15184,7 +15184,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -15206,7 +15206,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -15228,7 +15228,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -15250,7 +15250,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -15272,7 +15272,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -15294,7 +15294,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -15316,7 +15316,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -15338,7 +15338,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -15360,7 +15360,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -15382,7 +15382,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -15404,7 +15404,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -15426,7 +15426,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -15448,7 +15448,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -15470,7 +15470,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -15492,7 +15492,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -15514,7 +15514,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -15536,7 +15536,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -15558,7 +15558,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -15580,7 +15580,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -15602,7 +15602,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -15624,7 +15624,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -15646,7 +15646,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -15668,7 +15668,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -15690,7 +15690,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -15712,7 +15712,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -15734,7 +15734,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -15756,7 +15756,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -15778,7 +15778,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -15800,7 +15800,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -15822,7 +15822,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -15844,7 +15844,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -15866,7 +15866,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -15888,7 +15888,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -15910,7 +15910,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15932,7 +15932,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15954,7 +15954,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15976,7 +15976,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15998,7 +15998,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -16020,7 +16020,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -16042,7 +16042,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -16064,7 +16064,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -16086,7 +16086,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -16108,7 +16108,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -16130,7 +16130,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -16152,7 +16152,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -16174,7 +16174,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -16196,7 +16196,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -16218,7 +16218,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -16240,7 +16240,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -16262,7 +16262,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -16284,7 +16284,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -16306,7 +16306,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -16328,7 +16328,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -16350,7 +16350,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -16372,7 +16372,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -16394,7 +16394,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -16416,7 +16416,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -16438,7 +16438,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -16460,7 +16460,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -16482,7 +16482,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -16504,7 +16504,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -16526,7 +16526,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -16548,7 +16548,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -16570,7 +16570,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -16592,7 +16592,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -16614,7 +16614,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -16636,7 +16636,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -16658,7 +16658,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -16680,7 +16680,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -16702,7 +16702,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -16724,7 +16724,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -16746,7 +16746,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -16768,7 +16768,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -16790,7 +16790,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -16812,7 +16812,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -16834,7 +16834,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -16856,7 +16856,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -16878,7 +16878,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -16900,7 +16900,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -16922,7 +16922,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16944,7 +16944,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16966,7 +16966,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16988,7 +16988,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -17010,7 +17010,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -17032,7 +17032,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -17054,7 +17054,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -17076,7 +17076,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -17098,7 +17098,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -17120,7 +17120,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -17142,7 +17142,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -17164,7 +17164,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -17186,7 +17186,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -17208,7 +17208,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -17230,7 +17230,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -17252,7 +17252,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -17274,7 +17274,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -17296,7 +17296,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -17318,7 +17318,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -17340,7 +17340,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -17362,7 +17362,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -17384,7 +17384,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -17406,7 +17406,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -17428,29 +17428,29 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
       </c>
-      <c r="B278" s="17" t="str">
+      <c r="B278" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I279</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C278" s="48" t="str">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="C278" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J279</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D278" s="48" t="str">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="D278" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K279</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E278" s="5" t="str">
+        <v>4.4600000000000001E-2</v>
+      </c>
+      <c r="E278" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L279</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.7100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -17472,7 +17472,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -17494,7 +17494,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -17516,7 +17516,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -17538,7 +17538,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -17560,7 +17560,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -17582,7 +17582,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -17604,7 +17604,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -17626,7 +17626,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -17648,7 +17648,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -17670,7 +17670,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -17692,7 +17692,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -17714,7 +17714,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -17736,7 +17736,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -17758,7 +17758,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -17780,7 +17780,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -17802,7 +17802,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -17824,7 +17824,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -17846,7 +17846,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -17868,7 +17868,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -17890,7 +17890,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -17912,7 +17912,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17934,7 +17934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17956,7 +17956,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17978,7 +17978,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -18000,7 +18000,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -18022,7 +18022,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -18044,7 +18044,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -18066,7 +18066,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -18088,7 +18088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -18110,7 +18110,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -18132,7 +18132,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -18154,7 +18154,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -18176,7 +18176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -18198,7 +18198,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -18220,7 +18220,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -18242,7 +18242,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -18264,7 +18264,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -18286,7 +18286,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -18308,7 +18308,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -18330,7 +18330,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -18352,7 +18352,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -18374,7 +18374,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -18396,7 +18396,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -18418,7 +18418,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -18440,7 +18440,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -18462,7 +18462,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -18484,7 +18484,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -18506,7 +18506,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -18528,7 +18528,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -18550,7 +18550,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -18572,7 +18572,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -18594,7 +18594,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -18616,7 +18616,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -18638,7 +18638,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -18660,7 +18660,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -18682,7 +18682,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -18704,7 +18704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -18726,7 +18726,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -18748,7 +18748,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -18770,7 +18770,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -18792,7 +18792,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -18814,7 +18814,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -18836,7 +18836,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -18858,7 +18858,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -18880,7 +18880,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -18902,7 +18902,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -18924,7 +18924,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18946,7 +18946,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18968,7 +18968,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18990,7 +18990,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -19012,7 +19012,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -19034,7 +19034,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -19056,7 +19056,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -19078,7 +19078,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -19100,7 +19100,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -19122,7 +19122,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -19144,7 +19144,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -19166,7 +19166,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -19188,7 +19188,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -19210,7 +19210,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -19232,7 +19232,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -19254,7 +19254,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -19276,7 +19276,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -19298,7 +19298,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -19320,7 +19320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -19342,7 +19342,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -19364,7 +19364,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -19386,7 +19386,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -19408,7 +19408,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -19430,7 +19430,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -19452,37 +19452,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -19499,17 +19499,17 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -19518,14 +19518,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -19534,7 +19534,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -19543,7 +19543,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -19560,7 +19560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -19582,7 +19582,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -19604,7 +19604,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -19626,7 +19626,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -19648,7 +19648,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -19670,13 +19670,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -19685,7 +19685,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -19694,12 +19694,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -19708,7 +19708,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -19725,7 +19725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -19749,7 +19749,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -19773,7 +19773,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -19797,7 +19797,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -19821,7 +19821,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -19829,7 +19829,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -19837,7 +19837,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -19847,7 +19847,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -19857,7 +19857,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -19897,7 +19897,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -19919,7 +19919,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19941,7 +19941,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19963,7 +19963,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19971,7 +19971,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19979,7 +19979,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19989,7 +19989,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19999,7 +19999,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -20015,7 +20015,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -20035,7 +20035,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -20055,7 +20055,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -20075,7 +20075,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -20095,7 +20095,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -20104,7 +20104,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -20115,7 +20115,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -20126,7 +20126,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -20149,7 +20149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -20184,7 +20184,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -20219,7 +20219,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -20254,7 +20254,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -20311,193 +20311,193 @@
       <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="str">
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -20667,7 +20667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -20801,7 +20801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20975,7 +20975,7 @@
         <v>103.45</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -21149,7 +21149,7 @@
         <v>108.31</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -21323,7 +21323,7 @@
         <v>113.18</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -21497,7 +21497,7 @@
         <v>118.04</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -21671,7 +21671,7 @@
         <v>121.04</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -21845,7 +21845,7 @@
         <v>124.05</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -22019,7 +22019,7 @@
         <v>125.72</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -22193,7 +22193,7 @@
         <v>127.39</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -22367,7 +22367,7 @@
         <v>129.06</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -22541,7 +22541,7 @@
         <v>129.35</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -22715,7 +22715,7 @@
         <v>129.63999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -22889,7 +22889,7 @@
         <v>129.93</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -23063,7 +23063,7 @@
         <v>130.22</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -23237,7 +23237,7 @@
         <v>130.51</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>130.80000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -23585,7 +23585,7 @@
         <v>131.09</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -23759,7 +23759,7 @@
         <v>131.38</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23933,7 +23933,7 @@
         <v>131.66999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -24107,7 +24107,7 @@
         <v>131.96</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -24281,7 +24281,7 @@
         <v>132.25</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -24455,7 +24455,7 @@
         <v>132.54</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -24629,7 +24629,7 @@
         <v>132.83000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -24803,7 +24803,7 @@
         <v>133.12</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24977,7 +24977,7 @@
         <v>133.41</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -25151,7 +25151,7 @@
         <v>133.69999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -25325,7 +25325,7 @@
         <v>133.99</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -25499,7 +25499,7 @@
         <v>134.28</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>134.57</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -25847,7 +25847,7 @@
         <v>134.86000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>135.15</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26224,7 +26224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26245,7 +26245,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
+                <xdr:colOff>488950</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-08
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EA3C8C-0C62-47E1-82BB-57B7A4B78691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDB39B4-671D-4E9F-B246-EB26AA9E3D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>488950</xdr:colOff>
+          <xdr:colOff>485775</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -9580,17 +9580,17 @@
           <cell r="H284">
             <v>45937</v>
           </cell>
-          <cell r="I284" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J284" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K284" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L284" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I284">
+            <v>3.9699999999999999E-2</v>
+          </cell>
+          <cell r="J284">
+            <v>4.2599999999999999E-2</v>
+          </cell>
+          <cell r="K284">
+            <v>4.4999999999999998E-2</v>
+          </cell>
+          <cell r="L284">
+            <v>4.7399999999999998E-2</v>
           </cell>
         </row>
         <row r="285">
@@ -11352,20 +11352,20 @@
   <dimension ref="A1:E380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E281" sqref="E281"/>
+      <pane ySplit="3" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B283" sqref="B283"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -11374,7 +11374,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -11383,7 +11383,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -11422,7 +11422,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -11444,7 +11444,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -11466,7 +11466,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -11488,7 +11488,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -11510,7 +11510,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -11532,7 +11532,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -11554,7 +11554,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -11576,7 +11576,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -11598,7 +11598,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -11620,7 +11620,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -11642,7 +11642,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -11664,7 +11664,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -11686,7 +11686,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -11708,7 +11708,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -11730,7 +11730,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -11752,7 +11752,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -11774,7 +11774,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -11796,7 +11796,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -11818,7 +11818,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -11840,7 +11840,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -11862,7 +11862,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -11884,7 +11884,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -11906,7 +11906,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -11928,7 +11928,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11950,7 +11950,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11972,7 +11972,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11994,7 +11994,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -12016,7 +12016,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -12038,7 +12038,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -12060,7 +12060,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -12082,7 +12082,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -12104,7 +12104,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -12126,7 +12126,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -12148,7 +12148,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -12170,7 +12170,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -12192,7 +12192,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -12214,7 +12214,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -12236,7 +12236,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -12258,7 +12258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -12280,7 +12280,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -12302,7 +12302,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -12324,7 +12324,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -12346,7 +12346,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -12368,7 +12368,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -12390,7 +12390,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -12412,7 +12412,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -12434,7 +12434,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -12456,7 +12456,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -12478,7 +12478,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -12500,7 +12500,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -12522,7 +12522,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -12544,7 +12544,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -12566,7 +12566,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -12588,7 +12588,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -12610,7 +12610,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -12632,7 +12632,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -12654,7 +12654,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -12676,7 +12676,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -12698,7 +12698,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -12720,7 +12720,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -12742,7 +12742,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -12764,7 +12764,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -12786,7 +12786,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -12808,7 +12808,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -12830,7 +12830,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -12852,7 +12852,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -12874,7 +12874,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -12896,7 +12896,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -12918,7 +12918,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12940,7 +12940,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12962,7 +12962,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12984,7 +12984,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -13006,7 +13006,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -13028,7 +13028,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -13050,7 +13050,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -13072,7 +13072,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -13094,7 +13094,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -13116,7 +13116,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -13138,7 +13138,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -13160,7 +13160,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -13182,7 +13182,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -13204,7 +13204,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -13226,7 +13226,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -13248,7 +13248,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -13270,7 +13270,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -13292,7 +13292,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -13314,7 +13314,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -13336,7 +13336,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -13358,7 +13358,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -13380,7 +13380,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -13402,7 +13402,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -13424,7 +13424,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -13446,7 +13446,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -13468,7 +13468,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -13490,7 +13490,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -13512,7 +13512,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -13534,7 +13534,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -13556,7 +13556,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -13578,7 +13578,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -13600,7 +13600,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -13622,7 +13622,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -13644,7 +13644,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -13666,7 +13666,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -13688,7 +13688,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -13710,7 +13710,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -13732,7 +13732,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -13754,7 +13754,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -13776,7 +13776,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -13798,7 +13798,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -13820,7 +13820,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -13842,7 +13842,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -13864,7 +13864,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -13886,7 +13886,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -13908,7 +13908,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13930,7 +13930,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13952,7 +13952,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13974,7 +13974,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13996,7 +13996,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -14018,7 +14018,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -14040,7 +14040,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -14062,7 +14062,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -14084,7 +14084,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -14106,7 +14106,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -14128,7 +14128,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -14150,7 +14150,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -14172,7 +14172,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -14194,7 +14194,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -14216,7 +14216,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -14238,7 +14238,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -14260,7 +14260,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -14282,7 +14282,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -14304,7 +14304,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -14326,7 +14326,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -14348,7 +14348,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -14370,7 +14370,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -14392,7 +14392,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -14414,7 +14414,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -14436,7 +14436,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -14458,7 +14458,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -14480,7 +14480,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -14502,7 +14502,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -14524,7 +14524,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -14546,7 +14546,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -14568,7 +14568,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -14590,7 +14590,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -14612,7 +14612,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -14634,7 +14634,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -14656,7 +14656,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -14678,7 +14678,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -14700,7 +14700,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -14722,7 +14722,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -14744,7 +14744,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -14766,7 +14766,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -14788,7 +14788,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -14810,7 +14810,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -14832,7 +14832,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -14854,7 +14854,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -14876,7 +14876,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -14898,7 +14898,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -14920,7 +14920,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14942,7 +14942,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14964,7 +14964,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14986,7 +14986,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -15008,7 +15008,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -15030,7 +15030,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -15052,7 +15052,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -15074,7 +15074,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -15096,7 +15096,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -15118,7 +15118,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -15140,7 +15140,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -15162,7 +15162,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -15184,7 +15184,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -15206,7 +15206,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -15228,7 +15228,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -15250,7 +15250,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -15272,7 +15272,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -15294,7 +15294,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -15316,7 +15316,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -15338,7 +15338,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -15360,7 +15360,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -15382,7 +15382,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -15404,7 +15404,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -15426,7 +15426,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -15448,7 +15448,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -15470,7 +15470,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -15492,7 +15492,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -15514,7 +15514,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -15536,7 +15536,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -15558,7 +15558,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -15580,7 +15580,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -15602,7 +15602,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -15624,7 +15624,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -15646,7 +15646,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -15668,7 +15668,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -15690,7 +15690,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -15712,7 +15712,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -15734,7 +15734,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -15756,7 +15756,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -15778,7 +15778,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -15800,7 +15800,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -15822,7 +15822,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -15844,7 +15844,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -15866,7 +15866,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -15888,7 +15888,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -15910,7 +15910,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15932,7 +15932,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15954,7 +15954,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15976,7 +15976,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15998,7 +15998,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -16020,7 +16020,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -16042,7 +16042,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -16064,7 +16064,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -16086,7 +16086,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -16108,7 +16108,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -16130,7 +16130,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -16152,7 +16152,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -16174,7 +16174,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -16196,7 +16196,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -16218,7 +16218,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -16240,7 +16240,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -16262,7 +16262,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -16284,7 +16284,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -16306,7 +16306,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -16328,7 +16328,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -16350,7 +16350,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -16372,7 +16372,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -16394,7 +16394,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -16416,7 +16416,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -16438,7 +16438,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -16460,7 +16460,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -16482,7 +16482,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -16504,7 +16504,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -16526,7 +16526,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -16548,7 +16548,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -16570,7 +16570,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -16592,7 +16592,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -16614,7 +16614,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -16636,7 +16636,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -16658,7 +16658,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -16680,7 +16680,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -16702,7 +16702,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -16724,7 +16724,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -16746,7 +16746,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -16768,7 +16768,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -16790,7 +16790,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -16812,7 +16812,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -16834,7 +16834,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -16856,7 +16856,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -16878,7 +16878,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -16900,7 +16900,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -16922,7 +16922,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16944,7 +16944,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16966,7 +16966,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16988,7 +16988,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -17010,7 +17010,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -17032,7 +17032,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -17054,7 +17054,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -17076,7 +17076,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -17098,7 +17098,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -17120,7 +17120,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -17142,7 +17142,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -17164,7 +17164,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -17186,7 +17186,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -17208,7 +17208,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -17230,7 +17230,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -17252,7 +17252,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -17274,7 +17274,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -17296,7 +17296,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -17318,7 +17318,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -17340,7 +17340,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -17362,7 +17362,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -17384,7 +17384,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -17406,7 +17406,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -17428,7 +17428,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -17450,7 +17450,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -17472,7 +17472,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -17494,7 +17494,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -17516,7 +17516,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -17538,29 +17538,29 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
       </c>
-      <c r="B283" s="17" t="str">
+      <c r="B283" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I284</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C283" s="48" t="str">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C283" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J284</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D283" s="48" t="str">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="D283" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K284</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E283" s="5" t="str">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E283" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L284</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.7399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -17582,7 +17582,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -17604,7 +17604,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -17626,7 +17626,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -17648,7 +17648,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -17670,7 +17670,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -17692,7 +17692,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -17714,7 +17714,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -17736,7 +17736,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -17758,7 +17758,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -17780,7 +17780,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -17802,7 +17802,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -17824,7 +17824,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -17846,7 +17846,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -17868,7 +17868,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -17890,7 +17890,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -17912,7 +17912,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17934,7 +17934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17956,7 +17956,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17978,7 +17978,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -18000,7 +18000,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -18022,7 +18022,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -18044,7 +18044,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -18066,7 +18066,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -18088,7 +18088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -18110,7 +18110,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -18132,7 +18132,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -18154,7 +18154,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -18176,7 +18176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -18198,7 +18198,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -18220,7 +18220,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -18242,7 +18242,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -18264,7 +18264,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -18286,7 +18286,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -18308,7 +18308,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -18330,7 +18330,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -18352,7 +18352,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -18374,7 +18374,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -18396,7 +18396,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -18418,7 +18418,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -18440,7 +18440,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -18462,7 +18462,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -18484,7 +18484,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -18506,7 +18506,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -18528,7 +18528,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -18550,7 +18550,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -18572,7 +18572,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -18594,7 +18594,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -18616,7 +18616,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -18638,7 +18638,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -18660,7 +18660,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -18682,7 +18682,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -18704,7 +18704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -18726,7 +18726,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -18748,7 +18748,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -18770,7 +18770,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -18792,7 +18792,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -18814,7 +18814,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -18836,7 +18836,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -18858,7 +18858,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -18880,7 +18880,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -18902,7 +18902,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -18924,7 +18924,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18946,7 +18946,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18968,7 +18968,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18990,7 +18990,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -19012,7 +19012,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -19034,7 +19034,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -19056,7 +19056,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -19078,7 +19078,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -19100,7 +19100,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -19122,7 +19122,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -19144,7 +19144,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -19166,7 +19166,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -19188,7 +19188,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -19210,7 +19210,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -19232,7 +19232,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -19254,7 +19254,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -19276,7 +19276,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -19298,7 +19298,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -19320,7 +19320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -19342,7 +19342,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -19364,7 +19364,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -19386,7 +19386,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -19408,7 +19408,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -19430,7 +19430,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -19452,37 +19452,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -19503,13 +19503,13 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -19518,14 +19518,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -19534,7 +19534,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -19543,7 +19543,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -19560,7 +19560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -19582,7 +19582,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -19604,7 +19604,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -19626,7 +19626,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -19648,7 +19648,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -19670,13 +19670,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -19685,7 +19685,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -19694,12 +19694,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -19708,7 +19708,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -19725,7 +19725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -19749,7 +19749,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -19773,7 +19773,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -19797,7 +19797,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -19821,7 +19821,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -19829,7 +19829,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -19837,7 +19837,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -19847,7 +19847,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -19857,7 +19857,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -19897,7 +19897,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -19919,7 +19919,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19941,7 +19941,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19963,7 +19963,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19971,7 +19971,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19979,7 +19979,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19989,7 +19989,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19999,7 +19999,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -20015,7 +20015,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -20035,7 +20035,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -20055,7 +20055,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -20075,7 +20075,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -20095,7 +20095,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -20104,7 +20104,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -20115,7 +20115,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -20126,7 +20126,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -20149,7 +20149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -20184,7 +20184,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -20219,7 +20219,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -20254,7 +20254,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -20311,193 +20311,193 @@
       <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="str">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -20667,7 +20667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -20801,7 +20801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20975,7 +20975,7 @@
         <v>103.45</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -21149,7 +21149,7 @@
         <v>108.31</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -21323,7 +21323,7 @@
         <v>113.18</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -21497,7 +21497,7 @@
         <v>118.04</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -21671,7 +21671,7 @@
         <v>121.04</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -21845,7 +21845,7 @@
         <v>124.05</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -22019,7 +22019,7 @@
         <v>125.72</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -22193,7 +22193,7 @@
         <v>127.39</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -22367,7 +22367,7 @@
         <v>129.06</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -22541,7 +22541,7 @@
         <v>129.35</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -22715,7 +22715,7 @@
         <v>129.63999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -22889,7 +22889,7 @@
         <v>129.93</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -23063,7 +23063,7 @@
         <v>130.22</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -23237,7 +23237,7 @@
         <v>130.51</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>130.80000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -23585,7 +23585,7 @@
         <v>131.09</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -23759,7 +23759,7 @@
         <v>131.38</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23933,7 +23933,7 @@
         <v>131.66999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -24107,7 +24107,7 @@
         <v>131.96</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -24281,7 +24281,7 @@
         <v>132.25</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -24455,7 +24455,7 @@
         <v>132.54</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -24629,7 +24629,7 @@
         <v>132.83000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -24803,7 +24803,7 @@
         <v>133.12</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24977,7 +24977,7 @@
         <v>133.41</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -25151,7 +25151,7 @@
         <v>133.69999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -25325,7 +25325,7 @@
         <v>133.99</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -25499,7 +25499,7 @@
         <v>134.28</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>134.57</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -25847,7 +25847,7 @@
         <v>134.86000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>135.15</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26224,7 +26224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26245,7 +26245,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>488950</xdr:colOff>
+                <xdr:colOff>485775</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-09
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDB39B4-671D-4E9F-B246-EB26AA9E3D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2CF033-CCCA-43EA-BCC0-49D64092325D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31425" yWindow="0" windowWidth="24675" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9597,17 +9597,17 @@
           <cell r="H285">
             <v>45938</v>
           </cell>
-          <cell r="I285" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J285" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K285" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L285" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I285">
+            <v>3.9399999999999998E-2</v>
+          </cell>
+          <cell r="J285">
+            <v>4.24E-2</v>
+          </cell>
+          <cell r="K285">
+            <v>4.4699999999999997E-2</v>
+          </cell>
+          <cell r="L285">
+            <v>4.7199999999999999E-2</v>
           </cell>
         </row>
         <row r="286">
@@ -17565,21 +17565,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
       </c>
-      <c r="B284" s="17" t="str">
+      <c r="B284" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I285</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C284" s="48" t="str">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="C284" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J285</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D284" s="48" t="str">
+        <v>4.24E-2</v>
+      </c>
+      <c r="D284" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K285</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E284" s="5" t="str">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="E284" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L285</f>
-        <v xml:space="preserve"> </v>
+        <v>4.7199999999999999E-2</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -20320,182 +20320,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="str" cm="1">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="str">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-10
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2CF033-CCCA-43EA-BCC0-49D64092325D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0DE82D-D99C-4ED7-A059-F0077C0ADCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31425" yWindow="0" windowWidth="24675" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
+          <xdr:colOff>488950</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -9614,17 +9614,17 @@
           <cell r="H286">
             <v>45939</v>
           </cell>
-          <cell r="I286" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J286" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K286" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L286" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I286">
+            <v>3.95E-2</v>
+          </cell>
+          <cell r="J286">
+            <v>4.24E-2</v>
+          </cell>
+          <cell r="K286">
+            <v>4.48E-2</v>
+          </cell>
+          <cell r="L286">
+            <v>4.7199999999999999E-2</v>
           </cell>
         </row>
         <row r="287">
@@ -11353,19 +11353,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B283" sqref="B283"/>
+      <selection pane="bottomLeft" activeCell="H279" sqref="H279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -11374,7 +11374,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -11383,7 +11383,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -11422,7 +11422,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -11444,7 +11444,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -11466,7 +11466,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -11488,7 +11488,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -11510,7 +11510,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -11532,7 +11532,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -11554,7 +11554,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -11576,7 +11576,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -11598,7 +11598,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -11620,7 +11620,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -11642,7 +11642,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -11664,7 +11664,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -11686,7 +11686,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -11708,7 +11708,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -11730,7 +11730,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -11752,7 +11752,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -11774,7 +11774,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -11796,7 +11796,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -11818,7 +11818,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -11840,7 +11840,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -11862,7 +11862,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -11884,7 +11884,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -11906,7 +11906,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -11928,7 +11928,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11950,7 +11950,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11972,7 +11972,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11994,7 +11994,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -12016,7 +12016,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -12038,7 +12038,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -12060,7 +12060,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -12082,7 +12082,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -12104,7 +12104,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -12126,7 +12126,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -12148,7 +12148,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -12170,7 +12170,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -12192,7 +12192,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -12214,7 +12214,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -12236,7 +12236,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -12258,7 +12258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -12280,7 +12280,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -12302,7 +12302,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -12324,7 +12324,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -12346,7 +12346,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -12368,7 +12368,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -12390,7 +12390,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -12412,7 +12412,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -12434,7 +12434,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -12456,7 +12456,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -12478,7 +12478,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -12500,7 +12500,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -12522,7 +12522,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -12544,7 +12544,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -12566,7 +12566,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -12588,7 +12588,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -12610,7 +12610,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -12632,7 +12632,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -12654,7 +12654,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -12676,7 +12676,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -12698,7 +12698,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -12720,7 +12720,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -12742,7 +12742,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -12764,7 +12764,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -12786,7 +12786,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -12808,7 +12808,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -12830,7 +12830,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -12852,7 +12852,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -12874,7 +12874,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -12896,7 +12896,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -12918,7 +12918,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12940,7 +12940,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12962,7 +12962,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12984,7 +12984,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -13006,7 +13006,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -13028,7 +13028,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -13050,7 +13050,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -13072,7 +13072,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -13094,7 +13094,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -13116,7 +13116,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -13138,7 +13138,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -13160,7 +13160,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -13182,7 +13182,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -13204,7 +13204,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -13226,7 +13226,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -13248,7 +13248,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -13270,7 +13270,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -13292,7 +13292,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -13314,7 +13314,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -13336,7 +13336,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -13358,7 +13358,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -13380,7 +13380,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -13402,7 +13402,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -13424,7 +13424,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -13446,7 +13446,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -13468,7 +13468,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -13490,7 +13490,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -13512,7 +13512,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -13534,7 +13534,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -13556,7 +13556,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -13578,7 +13578,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -13600,7 +13600,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -13622,7 +13622,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -13644,7 +13644,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -13666,7 +13666,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -13688,7 +13688,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -13710,7 +13710,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -13732,7 +13732,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -13754,7 +13754,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -13776,7 +13776,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -13798,7 +13798,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -13820,7 +13820,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -13842,7 +13842,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -13864,7 +13864,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -13886,7 +13886,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -13908,7 +13908,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13930,7 +13930,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13952,7 +13952,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13974,7 +13974,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13996,7 +13996,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -14018,7 +14018,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -14040,7 +14040,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -14062,7 +14062,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -14084,7 +14084,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -14106,7 +14106,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -14128,7 +14128,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -14150,7 +14150,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -14172,7 +14172,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -14194,7 +14194,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -14216,7 +14216,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -14238,7 +14238,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -14260,7 +14260,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -14282,7 +14282,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -14304,7 +14304,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -14326,7 +14326,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -14348,7 +14348,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -14370,7 +14370,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -14392,7 +14392,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -14414,7 +14414,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -14436,7 +14436,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -14458,7 +14458,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -14480,7 +14480,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -14502,7 +14502,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -14524,7 +14524,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -14546,7 +14546,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -14568,7 +14568,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -14590,7 +14590,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -14612,7 +14612,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -14634,7 +14634,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -14656,7 +14656,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -14678,7 +14678,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -14700,7 +14700,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -14722,7 +14722,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -14744,7 +14744,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -14766,7 +14766,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -14788,7 +14788,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -14810,7 +14810,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -14832,7 +14832,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -14854,7 +14854,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -14876,7 +14876,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -14898,7 +14898,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -14920,7 +14920,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14942,7 +14942,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14964,7 +14964,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14986,7 +14986,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -15008,7 +15008,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -15030,7 +15030,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -15052,7 +15052,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -15074,7 +15074,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -15096,7 +15096,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -15118,7 +15118,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -15140,7 +15140,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -15162,7 +15162,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -15184,7 +15184,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -15206,7 +15206,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -15228,7 +15228,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -15250,7 +15250,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -15272,7 +15272,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -15294,7 +15294,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -15316,7 +15316,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -15338,7 +15338,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -15360,7 +15360,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -15382,7 +15382,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -15404,7 +15404,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -15426,7 +15426,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -15448,7 +15448,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -15470,7 +15470,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -15492,7 +15492,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -15514,7 +15514,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -15536,7 +15536,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -15558,7 +15558,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -15580,7 +15580,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -15602,7 +15602,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -15624,7 +15624,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -15646,7 +15646,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -15668,7 +15668,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -15690,7 +15690,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -15712,7 +15712,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -15734,7 +15734,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -15756,7 +15756,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -15778,7 +15778,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -15800,7 +15800,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -15822,7 +15822,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -15844,7 +15844,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -15866,7 +15866,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -15888,7 +15888,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -15910,7 +15910,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15932,7 +15932,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15954,7 +15954,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15976,7 +15976,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15998,7 +15998,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -16020,7 +16020,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -16042,7 +16042,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -16064,7 +16064,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -16086,7 +16086,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -16108,7 +16108,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -16130,7 +16130,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -16152,7 +16152,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -16174,7 +16174,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -16196,7 +16196,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -16218,7 +16218,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -16240,7 +16240,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -16262,7 +16262,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -16284,7 +16284,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -16306,7 +16306,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -16328,7 +16328,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -16350,7 +16350,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -16372,7 +16372,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -16394,7 +16394,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -16416,7 +16416,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -16438,7 +16438,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -16460,7 +16460,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -16482,7 +16482,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -16504,7 +16504,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -16526,7 +16526,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -16548,7 +16548,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -16570,7 +16570,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -16592,7 +16592,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -16614,7 +16614,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -16636,7 +16636,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -16658,7 +16658,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -16680,7 +16680,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -16702,7 +16702,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -16724,7 +16724,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -16746,7 +16746,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -16768,7 +16768,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -16790,7 +16790,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -16812,7 +16812,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -16834,7 +16834,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -16856,7 +16856,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -16878,7 +16878,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -16900,7 +16900,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -16922,7 +16922,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16944,7 +16944,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16966,7 +16966,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16988,7 +16988,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -17010,7 +17010,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -17032,7 +17032,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -17054,7 +17054,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -17076,7 +17076,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -17098,7 +17098,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -17120,7 +17120,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -17142,7 +17142,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -17164,7 +17164,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -17186,7 +17186,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -17208,7 +17208,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -17230,7 +17230,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -17252,7 +17252,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -17274,7 +17274,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -17296,7 +17296,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -17318,7 +17318,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -17340,7 +17340,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -17362,7 +17362,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -17384,7 +17384,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -17406,7 +17406,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -17428,7 +17428,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -17450,7 +17450,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -17472,7 +17472,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -17494,7 +17494,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -17516,7 +17516,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -17538,7 +17538,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -17560,7 +17560,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -17582,29 +17582,29 @@
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
       </c>
-      <c r="B285" s="17" t="str">
+      <c r="B285" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I286</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C285" s="48" t="str">
+        <v>3.95E-2</v>
+      </c>
+      <c r="C285" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J286</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D285" s="48" t="str">
+        <v>4.24E-2</v>
+      </c>
+      <c r="D285" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K286</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E285" s="5" t="str">
+        <v>4.48E-2</v>
+      </c>
+      <c r="E285" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L286</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.7199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -17626,7 +17626,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -17648,7 +17648,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -17670,7 +17670,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -17692,7 +17692,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -17714,7 +17714,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -17736,7 +17736,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -17758,7 +17758,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -17780,7 +17780,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -17802,7 +17802,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -17824,7 +17824,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -17846,7 +17846,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -17868,7 +17868,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -17890,7 +17890,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -17912,7 +17912,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17934,7 +17934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17956,7 +17956,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17978,7 +17978,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -18000,7 +18000,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -18022,7 +18022,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -18044,7 +18044,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -18066,7 +18066,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -18088,7 +18088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -18110,7 +18110,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -18132,7 +18132,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -18154,7 +18154,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -18176,7 +18176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -18198,7 +18198,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -18220,7 +18220,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -18242,7 +18242,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -18264,7 +18264,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -18286,7 +18286,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -18308,7 +18308,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -18330,7 +18330,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -18352,7 +18352,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -18374,7 +18374,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -18396,7 +18396,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -18418,7 +18418,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -18440,7 +18440,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -18462,7 +18462,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -18484,7 +18484,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -18506,7 +18506,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -18528,7 +18528,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -18550,7 +18550,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -18572,7 +18572,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -18594,7 +18594,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -18616,7 +18616,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -18638,7 +18638,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -18660,7 +18660,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -18682,7 +18682,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -18704,7 +18704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -18726,7 +18726,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -18748,7 +18748,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -18770,7 +18770,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -18792,7 +18792,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -18814,7 +18814,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -18836,7 +18836,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -18858,7 +18858,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -18880,7 +18880,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -18902,7 +18902,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -18924,7 +18924,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18946,7 +18946,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18968,7 +18968,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18990,7 +18990,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -19012,7 +19012,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -19034,7 +19034,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -19056,7 +19056,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -19078,7 +19078,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -19100,7 +19100,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -19122,7 +19122,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -19144,7 +19144,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -19166,7 +19166,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -19188,7 +19188,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -19210,7 +19210,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -19232,7 +19232,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -19254,7 +19254,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -19276,7 +19276,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -19298,7 +19298,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -19320,7 +19320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -19342,7 +19342,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -19364,7 +19364,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -19386,7 +19386,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -19408,7 +19408,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -19430,7 +19430,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -19452,37 +19452,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -19503,13 +19503,13 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -19518,14 +19518,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -19534,7 +19534,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -19543,7 +19543,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -19560,7 +19560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -19582,7 +19582,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -19604,7 +19604,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -19626,7 +19626,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -19648,7 +19648,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -19670,13 +19670,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -19685,7 +19685,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -19694,12 +19694,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -19708,7 +19708,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -19725,7 +19725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -19749,7 +19749,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -19773,7 +19773,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -19797,7 +19797,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -19821,7 +19821,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -19829,7 +19829,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -19837,7 +19837,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -19847,7 +19847,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -19857,7 +19857,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -19897,7 +19897,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -19919,7 +19919,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19941,7 +19941,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19963,7 +19963,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19971,7 +19971,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19979,7 +19979,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19989,7 +19989,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19999,7 +19999,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -20015,7 +20015,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -20035,7 +20035,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -20055,7 +20055,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -20075,7 +20075,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -20095,7 +20095,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -20104,7 +20104,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -20115,7 +20115,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -20126,7 +20126,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -20149,7 +20149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -20184,7 +20184,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -20219,7 +20219,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -20254,7 +20254,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -20311,193 +20311,193 @@
       <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="str">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -20667,7 +20667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -20801,7 +20801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20975,7 +20975,7 @@
         <v>103.45</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -21149,7 +21149,7 @@
         <v>108.31</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -21323,7 +21323,7 @@
         <v>113.18</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -21497,7 +21497,7 @@
         <v>118.04</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -21671,7 +21671,7 @@
         <v>121.04</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -21845,7 +21845,7 @@
         <v>124.05</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -22019,7 +22019,7 @@
         <v>125.72</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -22193,7 +22193,7 @@
         <v>127.39</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -22367,7 +22367,7 @@
         <v>129.06</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -22541,7 +22541,7 @@
         <v>129.35</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -22715,7 +22715,7 @@
         <v>129.63999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -22889,7 +22889,7 @@
         <v>129.93</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -23063,7 +23063,7 @@
         <v>130.22</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -23237,7 +23237,7 @@
         <v>130.51</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>130.80000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -23585,7 +23585,7 @@
         <v>131.09</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -23759,7 +23759,7 @@
         <v>131.38</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23933,7 +23933,7 @@
         <v>131.66999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -24107,7 +24107,7 @@
         <v>131.96</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -24281,7 +24281,7 @@
         <v>132.25</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -24455,7 +24455,7 @@
         <v>132.54</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -24629,7 +24629,7 @@
         <v>132.83000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -24803,7 +24803,7 @@
         <v>133.12</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24977,7 +24977,7 @@
         <v>133.41</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -25151,7 +25151,7 @@
         <v>133.69999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -25325,7 +25325,7 @@
         <v>133.99</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -25499,7 +25499,7 @@
         <v>134.28</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>134.57</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -25847,7 +25847,7 @@
         <v>134.86000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>135.15</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26224,7 +26224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26245,7 +26245,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
+                <xdr:colOff>488950</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-18
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD814DCD-1149-4D43-82A4-E44D074537AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13AA02-BEAA-4CBA-BEDB-7A0052EF13C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9750,17 +9750,17 @@
           <cell r="H294">
             <v>45947</v>
           </cell>
-          <cell r="I294" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J294" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K294" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L294" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I294">
+            <v>3.8300000000000001E-2</v>
+          </cell>
+          <cell r="J294">
+            <v>4.1300000000000003E-2</v>
+          </cell>
+          <cell r="K294">
+            <v>4.3700000000000003E-2</v>
+          </cell>
+          <cell r="L294">
+            <v>4.6100000000000002E-2</v>
           </cell>
         </row>
         <row r="295">
@@ -17763,21 +17763,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
       </c>
-      <c r="B293" s="17" t="str">
+      <c r="B293" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I294</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C293" s="48" t="str">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="C293" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J294</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D293" s="48" t="str">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="D293" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K294</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E293" s="5" t="str">
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="E293" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L294</f>
-        <v xml:space="preserve"> </v>
+        <v>4.6100000000000002E-2</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.35">
@@ -20320,182 +20320,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="str" cm="1">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="str">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-21
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13AA02-BEAA-4CBA-BEDB-7A0052EF13C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6500ACF-0CEA-4FC1-B20C-A017799339EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9767,51 +9767,51 @@
           <cell r="H295">
             <v>45948</v>
           </cell>
-          <cell r="I295" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J295" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K295" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L295" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I295">
+            <v>3.8600000000000002E-2</v>
+          </cell>
+          <cell r="J295">
+            <v>4.1599999999999998E-2</v>
+          </cell>
+          <cell r="K295">
+            <v>4.3900000000000002E-2</v>
+          </cell>
+          <cell r="L295">
+            <v>4.6300000000000001E-2</v>
           </cell>
         </row>
         <row r="296">
           <cell r="H296">
             <v>45949</v>
           </cell>
-          <cell r="I296" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J296" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K296" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L296" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I296">
+            <v>3.8600000000000002E-2</v>
+          </cell>
+          <cell r="J296">
+            <v>4.1599999999999998E-2</v>
+          </cell>
+          <cell r="K296">
+            <v>4.3900000000000002E-2</v>
+          </cell>
+          <cell r="L296">
+            <v>4.6300000000000001E-2</v>
           </cell>
         </row>
         <row r="297">
           <cell r="H297">
             <v>45950</v>
           </cell>
-          <cell r="I297" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J297" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K297" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L297" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I297">
+            <v>3.8600000000000002E-2</v>
+          </cell>
+          <cell r="J297">
+            <v>4.1599999999999998E-2</v>
+          </cell>
+          <cell r="K297">
+            <v>4.3900000000000002E-2</v>
+          </cell>
+          <cell r="L297">
+            <v>4.6300000000000001E-2</v>
           </cell>
         </row>
         <row r="298">
@@ -11353,7 +11353,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H288" sqref="H288"/>
+      <selection pane="bottomLeft" activeCell="B295" sqref="B295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17785,21 +17785,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
       </c>
-      <c r="B294" s="17" t="str">
+      <c r="B294" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I295</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C294" s="48" t="str">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="C294" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J295</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D294" s="48" t="str">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="D294" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K295</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E294" s="5" t="str">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="E294" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L295</f>
-        <v xml:space="preserve"> </v>
+        <v>4.6300000000000001E-2</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.35">
@@ -17807,21 +17807,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
       </c>
-      <c r="B295" s="17" t="str">
+      <c r="B295" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I296</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C295" s="48" t="str">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="C295" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J296</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D295" s="48" t="str">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="D295" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K296</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E295" s="5" t="str">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="E295" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L296</f>
-        <v xml:space="preserve"> </v>
+        <v>4.6300000000000001E-2</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.35">
@@ -17829,21 +17829,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
       </c>
-      <c r="B296" s="17" t="str">
+      <c r="B296" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I297</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C296" s="48" t="str">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="C296" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J297</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D296" s="48" t="str">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="D296" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K297</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E296" s="5" t="str">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="E296" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L297</f>
-        <v xml:space="preserve"> </v>
+        <v>4.6300000000000001E-2</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-22
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6500ACF-0CEA-4FC1-B20C-A017799339EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0AC26A-F5D7-4EA8-BDD4-23F4D3A6FED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>488950</xdr:colOff>
+          <xdr:colOff>485775</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -9818,17 +9818,17 @@
           <cell r="H298">
             <v>45951</v>
           </cell>
-          <cell r="I298" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J298" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K298" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L298" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I298">
+            <v>3.8399999999999997E-2</v>
+          </cell>
+          <cell r="J298">
+            <v>4.1300000000000003E-2</v>
+          </cell>
+          <cell r="K298">
+            <v>4.36E-2</v>
+          </cell>
+          <cell r="L298">
+            <v>4.5999999999999999E-2</v>
           </cell>
         </row>
         <row r="299">
@@ -11352,20 +11352,20 @@
   <dimension ref="A1:E380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B295" sqref="B295"/>
+      <pane ySplit="3" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B297" sqref="B297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -11374,7 +11374,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -11383,7 +11383,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -11422,7 +11422,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -11444,7 +11444,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -11466,7 +11466,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -11488,7 +11488,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -11510,7 +11510,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -11532,7 +11532,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -11554,7 +11554,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -11576,7 +11576,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -11598,7 +11598,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -11620,7 +11620,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -11642,7 +11642,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -11664,7 +11664,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -11686,7 +11686,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -11708,7 +11708,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -11730,7 +11730,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -11752,7 +11752,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -11774,7 +11774,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -11796,7 +11796,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -11818,7 +11818,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -11840,7 +11840,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -11862,7 +11862,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -11884,7 +11884,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -11906,7 +11906,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -11928,7 +11928,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11950,7 +11950,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11972,7 +11972,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11994,7 +11994,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -12016,7 +12016,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -12038,7 +12038,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -12060,7 +12060,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -12082,7 +12082,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -12104,7 +12104,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -12126,7 +12126,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -12148,7 +12148,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -12170,7 +12170,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -12192,7 +12192,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -12214,7 +12214,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -12236,7 +12236,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -12258,7 +12258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -12280,7 +12280,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -12302,7 +12302,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -12324,7 +12324,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -12346,7 +12346,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -12368,7 +12368,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -12390,7 +12390,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -12412,7 +12412,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -12434,7 +12434,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -12456,7 +12456,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -12478,7 +12478,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -12500,7 +12500,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -12522,7 +12522,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -12544,7 +12544,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -12566,7 +12566,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -12588,7 +12588,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -12610,7 +12610,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -12632,7 +12632,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -12654,7 +12654,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -12676,7 +12676,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -12698,7 +12698,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -12720,7 +12720,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -12742,7 +12742,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -12764,7 +12764,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -12786,7 +12786,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -12808,7 +12808,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -12830,7 +12830,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -12852,7 +12852,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -12874,7 +12874,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -12896,7 +12896,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -12918,7 +12918,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12940,7 +12940,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12962,7 +12962,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12984,7 +12984,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -13006,7 +13006,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -13028,7 +13028,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -13050,7 +13050,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -13072,7 +13072,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -13094,7 +13094,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -13116,7 +13116,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -13138,7 +13138,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -13160,7 +13160,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -13182,7 +13182,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -13204,7 +13204,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -13226,7 +13226,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -13248,7 +13248,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -13270,7 +13270,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -13292,7 +13292,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -13314,7 +13314,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -13336,7 +13336,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -13358,7 +13358,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -13380,7 +13380,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -13402,7 +13402,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -13424,7 +13424,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -13446,7 +13446,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -13468,7 +13468,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -13490,7 +13490,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -13512,7 +13512,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -13534,7 +13534,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -13556,7 +13556,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -13578,7 +13578,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -13600,7 +13600,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -13622,7 +13622,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -13644,7 +13644,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -13666,7 +13666,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -13688,7 +13688,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -13710,7 +13710,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -13732,7 +13732,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -13754,7 +13754,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -13776,7 +13776,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -13798,7 +13798,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -13820,7 +13820,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -13842,7 +13842,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -13864,7 +13864,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -13886,7 +13886,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -13908,7 +13908,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13930,7 +13930,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13952,7 +13952,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13974,7 +13974,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13996,7 +13996,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -14018,7 +14018,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -14040,7 +14040,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -14062,7 +14062,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -14084,7 +14084,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -14106,7 +14106,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -14128,7 +14128,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -14150,7 +14150,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -14172,7 +14172,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -14194,7 +14194,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -14216,7 +14216,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -14238,7 +14238,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -14260,7 +14260,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -14282,7 +14282,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -14304,7 +14304,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -14326,7 +14326,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -14348,7 +14348,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -14370,7 +14370,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -14392,7 +14392,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -14414,7 +14414,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -14436,7 +14436,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -14458,7 +14458,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -14480,7 +14480,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -14502,7 +14502,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -14524,7 +14524,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -14546,7 +14546,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -14568,7 +14568,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -14590,7 +14590,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -14612,7 +14612,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -14634,7 +14634,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -14656,7 +14656,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -14678,7 +14678,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -14700,7 +14700,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -14722,7 +14722,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -14744,7 +14744,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -14766,7 +14766,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -14788,7 +14788,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -14810,7 +14810,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -14832,7 +14832,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -14854,7 +14854,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -14876,7 +14876,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -14898,7 +14898,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -14920,7 +14920,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14942,7 +14942,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14964,7 +14964,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14986,7 +14986,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -15008,7 +15008,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -15030,7 +15030,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -15052,7 +15052,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -15074,7 +15074,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -15096,7 +15096,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -15118,7 +15118,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -15140,7 +15140,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -15162,7 +15162,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -15184,7 +15184,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -15206,7 +15206,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -15228,7 +15228,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -15250,7 +15250,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -15272,7 +15272,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -15294,7 +15294,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -15316,7 +15316,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -15338,7 +15338,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -15360,7 +15360,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -15382,7 +15382,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -15404,7 +15404,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -15426,7 +15426,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -15448,7 +15448,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -15470,7 +15470,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -15492,7 +15492,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -15514,7 +15514,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -15536,7 +15536,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -15558,7 +15558,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -15580,7 +15580,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -15602,7 +15602,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -15624,7 +15624,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -15646,7 +15646,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -15668,7 +15668,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -15690,7 +15690,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -15712,7 +15712,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -15734,7 +15734,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -15756,7 +15756,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -15778,7 +15778,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -15800,7 +15800,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -15822,7 +15822,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -15844,7 +15844,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -15866,7 +15866,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -15888,7 +15888,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -15910,7 +15910,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15932,7 +15932,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15954,7 +15954,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15976,7 +15976,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15998,7 +15998,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -16020,7 +16020,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -16042,7 +16042,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -16064,7 +16064,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -16086,7 +16086,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -16108,7 +16108,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -16130,7 +16130,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -16152,7 +16152,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -16174,7 +16174,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -16196,7 +16196,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -16218,7 +16218,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -16240,7 +16240,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -16262,7 +16262,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -16284,7 +16284,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -16306,7 +16306,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -16328,7 +16328,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -16350,7 +16350,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -16372,7 +16372,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -16394,7 +16394,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -16416,7 +16416,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -16438,7 +16438,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -16460,7 +16460,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -16482,7 +16482,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -16504,7 +16504,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -16526,7 +16526,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -16548,7 +16548,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -16570,7 +16570,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -16592,7 +16592,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -16614,7 +16614,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -16636,7 +16636,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -16658,7 +16658,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -16680,7 +16680,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -16702,7 +16702,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -16724,7 +16724,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -16746,7 +16746,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -16768,7 +16768,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -16790,7 +16790,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -16812,7 +16812,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -16834,7 +16834,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -16856,7 +16856,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -16878,7 +16878,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -16900,7 +16900,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -16922,7 +16922,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16944,7 +16944,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16966,7 +16966,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16988,7 +16988,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -17010,7 +17010,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -17032,7 +17032,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -17054,7 +17054,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -17076,7 +17076,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -17098,7 +17098,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -17120,7 +17120,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -17142,7 +17142,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -17164,7 +17164,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -17186,7 +17186,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -17208,7 +17208,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -17230,7 +17230,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -17252,7 +17252,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -17274,7 +17274,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -17296,7 +17296,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -17318,7 +17318,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -17340,7 +17340,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -17362,7 +17362,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -17384,7 +17384,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -17406,7 +17406,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -17428,7 +17428,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -17450,7 +17450,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -17472,7 +17472,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -17494,7 +17494,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -17516,7 +17516,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -17538,7 +17538,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -17560,7 +17560,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -17582,7 +17582,7 @@
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -17604,7 +17604,7 @@
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -17626,7 +17626,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -17648,7 +17648,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -17670,7 +17670,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -17692,7 +17692,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -17714,7 +17714,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -17736,7 +17736,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -17758,7 +17758,7 @@
         <v>4.6399999999999997E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -17780,7 +17780,7 @@
         <v>4.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -17802,7 +17802,7 @@
         <v>4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -17824,7 +17824,7 @@
         <v>4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -17846,29 +17846,29 @@
         <v>4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
       </c>
-      <c r="B297" s="17" t="str">
+      <c r="B297" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I298</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C297" s="48" t="str">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="C297" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J298</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D297" s="48" t="str">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="D297" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K298</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E297" s="5" t="str">
+        <v>4.36E-2</v>
+      </c>
+      <c r="E297" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L298</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -17890,7 +17890,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
@@ -17912,7 +17912,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17934,7 +17934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17956,7 +17956,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17978,7 +17978,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -18000,7 +18000,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -18022,7 +18022,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -18044,7 +18044,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -18066,7 +18066,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -18088,7 +18088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -18110,7 +18110,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -18132,7 +18132,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -18154,7 +18154,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -18176,7 +18176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -18198,7 +18198,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -18220,7 +18220,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -18242,7 +18242,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -18264,7 +18264,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -18286,7 +18286,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -18308,7 +18308,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -18330,7 +18330,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -18352,7 +18352,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -18374,7 +18374,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -18396,7 +18396,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -18418,7 +18418,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -18440,7 +18440,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -18462,7 +18462,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -18484,7 +18484,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -18506,7 +18506,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -18528,7 +18528,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -18550,7 +18550,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -18572,7 +18572,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -18594,7 +18594,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -18616,7 +18616,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -18638,7 +18638,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -18660,7 +18660,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -18682,7 +18682,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -18704,7 +18704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -18726,7 +18726,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -18748,7 +18748,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -18770,7 +18770,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -18792,7 +18792,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -18814,7 +18814,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -18836,7 +18836,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -18858,7 +18858,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -18880,7 +18880,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -18902,7 +18902,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -18924,7 +18924,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18946,7 +18946,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18968,7 +18968,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18990,7 +18990,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -19012,7 +19012,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -19034,7 +19034,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -19056,7 +19056,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -19078,7 +19078,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -19100,7 +19100,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -19122,7 +19122,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -19144,7 +19144,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -19166,7 +19166,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -19188,7 +19188,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -19210,7 +19210,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -19232,7 +19232,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -19254,7 +19254,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -19276,7 +19276,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -19298,7 +19298,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -19320,7 +19320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -19342,7 +19342,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -19364,7 +19364,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -19386,7 +19386,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -19408,7 +19408,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -19430,7 +19430,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -19452,37 +19452,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -19503,13 +19503,13 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -19518,14 +19518,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -19534,7 +19534,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -19543,7 +19543,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -19560,7 +19560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -19582,7 +19582,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -19604,7 +19604,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -19626,7 +19626,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -19648,7 +19648,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -19670,13 +19670,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -19685,7 +19685,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -19694,12 +19694,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -19708,7 +19708,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -19725,7 +19725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -19749,7 +19749,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -19773,7 +19773,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -19797,7 +19797,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -19821,7 +19821,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -19829,7 +19829,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -19837,7 +19837,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -19847,7 +19847,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -19857,7 +19857,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -19897,7 +19897,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -19919,7 +19919,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19941,7 +19941,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19963,7 +19963,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19971,7 +19971,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19979,7 +19979,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19989,7 +19989,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19999,7 +19999,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -20015,7 +20015,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -20035,7 +20035,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -20055,7 +20055,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -20075,7 +20075,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -20095,7 +20095,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -20104,7 +20104,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -20115,7 +20115,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -20126,7 +20126,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -20149,7 +20149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -20184,7 +20184,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -20219,7 +20219,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -20254,7 +20254,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -20311,193 +20311,193 @@
       <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="str">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -20667,7 +20667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -20801,7 +20801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20975,7 +20975,7 @@
         <v>103.45</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -21149,7 +21149,7 @@
         <v>108.31</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -21323,7 +21323,7 @@
         <v>113.18</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -21497,7 +21497,7 @@
         <v>118.04</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -21671,7 +21671,7 @@
         <v>121.04</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -21845,7 +21845,7 @@
         <v>124.05</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -22019,7 +22019,7 @@
         <v>125.72</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -22193,7 +22193,7 @@
         <v>127.39</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -22367,7 +22367,7 @@
         <v>129.06</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -22541,7 +22541,7 @@
         <v>129.35</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -22715,7 +22715,7 @@
         <v>129.63999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -22889,7 +22889,7 @@
         <v>129.93</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -23063,7 +23063,7 @@
         <v>130.22</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -23237,7 +23237,7 @@
         <v>130.51</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>130.80000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -23585,7 +23585,7 @@
         <v>131.09</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -23759,7 +23759,7 @@
         <v>131.38</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23933,7 +23933,7 @@
         <v>131.66999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -24107,7 +24107,7 @@
         <v>131.96</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -24281,7 +24281,7 @@
         <v>132.25</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -24455,7 +24455,7 @@
         <v>132.54</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -24629,7 +24629,7 @@
         <v>132.83000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -24803,7 +24803,7 @@
         <v>133.12</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24977,7 +24977,7 @@
         <v>133.41</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -25151,7 +25151,7 @@
         <v>133.69999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -25325,7 +25325,7 @@
         <v>133.99</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -25499,7 +25499,7 @@
         <v>134.28</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>134.57</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -25847,7 +25847,7 @@
         <v>134.86000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>135.15</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26224,7 +26224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26245,7 +26245,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>488950</xdr:colOff>
+                <xdr:colOff>485775</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-23
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0AC26A-F5D7-4EA8-BDD4-23F4D3A6FED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F01C13B-166D-47E1-8AB0-5273D6362813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34200" yWindow="2790" windowWidth="21075" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9835,17 +9835,17 @@
           <cell r="H299">
             <v>45952</v>
           </cell>
-          <cell r="I299" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J299" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K299" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L299" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I299">
+            <v>3.8300000000000001E-2</v>
+          </cell>
+          <cell r="J299">
+            <v>4.1099999999999998E-2</v>
+          </cell>
+          <cell r="K299">
+            <v>4.3400000000000001E-2</v>
+          </cell>
+          <cell r="L299">
+            <v>4.58E-2</v>
           </cell>
         </row>
         <row r="300">
@@ -17873,21 +17873,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
       </c>
-      <c r="B298" s="17" t="str">
+      <c r="B298" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I299</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C298" s="48" t="str">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="C298" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J299</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D298" s="48" t="str">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="D298" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K299</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E298" s="5" t="str">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="E298" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L299</f>
-        <v xml:space="preserve"> </v>
+        <v>4.58E-2</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -20320,182 +20320,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="str" cm="1">
+      <c r="A1" s="62" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="66" t="str" cm="1">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="64"/>
+      <c r="M1" s="62" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="68"/>
-      <c r="Y1" s="66" t="str" cm="1">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="Y1" s="62" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="68"/>
-      <c r="AK1" s="66" t="str" cm="1">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="64"/>
+      <c r="AK1" s="62" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="68"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="63"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="64"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="str">
+      <c r="A2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="64"/>
-      <c r="M2" s="62" t="str">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="67"/>
+      <c r="M2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="64"/>
-      <c r="Y2" s="62" t="str">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="67"/>
+      <c r="Y2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="64"/>
-      <c r="AK2" s="62" t="str">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="67"/>
+      <c r="AK2" s="65" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="64"/>
+      <c r="AL2" s="66"/>
+      <c r="AM2" s="66"/>
+      <c r="AN2" s="66"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="66"/>
+      <c r="AR2" s="66"/>
+      <c r="AS2" s="66"/>
+      <c r="AT2" s="66"/>
+      <c r="AU2" s="67"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="65" t="s">
+      <c r="N3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="65" t="s">
+      <c r="Z3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="65"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="65" t="s">
+      <c r="AL3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-24
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F01C13B-166D-47E1-8AB0-5273D6362813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45BE647-3F9C-4652-8FF7-4E6F5C97AC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34200" yWindow="2790" windowWidth="21075" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,15 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +586,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
+          <xdr:colOff>488950</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -9852,17 +9852,17 @@
           <cell r="H300">
             <v>45953</v>
           </cell>
-          <cell r="I300" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J300" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K300" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L300" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I300">
+            <v>3.8300000000000001E-2</v>
+          </cell>
+          <cell r="J300">
+            <v>4.1200000000000001E-2</v>
+          </cell>
+          <cell r="K300">
+            <v>4.3499999999999997E-2</v>
+          </cell>
+          <cell r="L300">
+            <v>4.5900000000000003E-2</v>
           </cell>
         </row>
         <row r="301">
@@ -11356,16 +11356,16 @@
       <selection pane="bottomLeft" activeCell="B297" sqref="B297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -11374,7 +11374,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -11383,7 +11383,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -11422,7 +11422,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -11444,7 +11444,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -11466,7 +11466,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -11488,7 +11488,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -11510,7 +11510,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -11532,7 +11532,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -11554,7 +11554,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -11576,7 +11576,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -11598,7 +11598,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -11620,7 +11620,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -11642,7 +11642,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>45669</v>
@@ -11664,7 +11664,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>45670</v>
@@ -11686,7 +11686,7 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>45671</v>
@@ -11708,7 +11708,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>45672</v>
@@ -11730,7 +11730,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>45673</v>
@@ -11752,7 +11752,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>45674</v>
@@ -11774,7 +11774,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>45675</v>
@@ -11796,7 +11796,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>45676</v>
@@ -11818,7 +11818,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>45677</v>
@@ -11840,7 +11840,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>45678</v>
@@ -11862,7 +11862,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>45679</v>
@@ -11884,7 +11884,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>45680</v>
@@ -11906,7 +11906,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>45681</v>
@@ -11928,7 +11928,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>45682</v>
@@ -11950,7 +11950,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>45683</v>
@@ -11972,7 +11972,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>45684</v>
@@ -11994,7 +11994,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>45685</v>
@@ -12016,7 +12016,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>45686</v>
@@ -12038,7 +12038,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>45687</v>
@@ -12060,7 +12060,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>45688</v>
@@ -12082,7 +12082,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>45689</v>
@@ -12104,7 +12104,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>45690</v>
@@ -12126,7 +12126,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>45691</v>
@@ -12148,7 +12148,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>45692</v>
@@ -12170,7 +12170,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>45693</v>
@@ -12192,7 +12192,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>45694</v>
@@ -12214,7 +12214,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>45695</v>
@@ -12236,7 +12236,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>45696</v>
@@ -12258,7 +12258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>45697</v>
@@ -12280,7 +12280,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>45698</v>
@@ -12302,7 +12302,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>45699</v>
@@ -12324,7 +12324,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>45700</v>
@@ -12346,7 +12346,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>45701</v>
@@ -12368,7 +12368,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>45702</v>
@@ -12390,7 +12390,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>45703</v>
@@ -12412,7 +12412,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>45704</v>
@@ -12434,7 +12434,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>45705</v>
@@ -12456,7 +12456,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>45706</v>
@@ -12478,7 +12478,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>45707</v>
@@ -12500,7 +12500,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>45708</v>
@@ -12522,7 +12522,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>45709</v>
@@ -12544,7 +12544,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>45710</v>
@@ -12566,7 +12566,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>45711</v>
@@ -12588,7 +12588,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>45712</v>
@@ -12610,7 +12610,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>45713</v>
@@ -12632,7 +12632,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>45714</v>
@@ -12654,7 +12654,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>45715</v>
@@ -12676,7 +12676,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>45716</v>
@@ -12698,7 +12698,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>45717</v>
@@ -12720,7 +12720,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>45718</v>
@@ -12742,7 +12742,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>45719</v>
@@ -12764,7 +12764,7 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>45720</v>
@@ -12786,7 +12786,7 @@
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>45721</v>
@@ -12808,7 +12808,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>45722</v>
@@ -12830,7 +12830,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>45723</v>
@@ -12852,7 +12852,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>45724</v>
@@ -12874,7 +12874,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>45725</v>
@@ -12896,7 +12896,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>45726</v>
@@ -12918,7 +12918,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>45727</v>
@@ -12940,7 +12940,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>45728</v>
@@ -12962,7 +12962,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>45729</v>
@@ -12984,7 +12984,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>45730</v>
@@ -13006,7 +13006,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>45731</v>
@@ -13028,7 +13028,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>45732</v>
@@ -13050,7 +13050,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>45733</v>
@@ -13072,7 +13072,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>45734</v>
@@ -13094,7 +13094,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>45735</v>
@@ -13116,7 +13116,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>45736</v>
@@ -13138,7 +13138,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>45737</v>
@@ -13160,7 +13160,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>45738</v>
@@ -13182,7 +13182,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>45739</v>
@@ -13204,7 +13204,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>45740</v>
@@ -13226,7 +13226,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>45741</v>
@@ -13248,7 +13248,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>45742</v>
@@ -13270,7 +13270,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>45743</v>
@@ -13292,7 +13292,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>45744</v>
@@ -13314,7 +13314,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>45745</v>
@@ -13336,7 +13336,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>45746</v>
@@ -13358,7 +13358,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>45747</v>
@@ -13380,7 +13380,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>45748</v>
@@ -13402,7 +13402,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>45749</v>
@@ -13424,7 +13424,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>45750</v>
@@ -13446,7 +13446,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>45751</v>
@@ -13468,7 +13468,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>45752</v>
@@ -13490,7 +13490,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>45753</v>
@@ -13512,7 +13512,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>45754</v>
@@ -13534,7 +13534,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>45755</v>
@@ -13556,7 +13556,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>45756</v>
@@ -13578,7 +13578,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>45757</v>
@@ -13600,7 +13600,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>45758</v>
@@ -13622,7 +13622,7 @@
         <v>5.3600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>45759</v>
@@ -13644,7 +13644,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>45760</v>
@@ -13666,7 +13666,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>45761</v>
@@ -13688,7 +13688,7 @@
         <v>5.3800000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>45762</v>
@@ -13710,7 +13710,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>45763</v>
@@ -13732,7 +13732,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>45764</v>
@@ -13754,7 +13754,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>45765</v>
@@ -13776,7 +13776,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>45766</v>
@@ -13798,7 +13798,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>45767</v>
@@ -13820,7 +13820,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>45768</v>
@@ -13842,7 +13842,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>45769</v>
@@ -13864,7 +13864,7 @@
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>45770</v>
@@ -13886,7 +13886,7 @@
         <v>5.2900000000000003E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>45771</v>
@@ -13908,7 +13908,7 @@
         <v>5.2200000000000003E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>45772</v>
@@ -13930,7 +13930,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>45773</v>
@@ -13952,7 +13952,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>45774</v>
@@ -13974,7 +13974,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>45775</v>
@@ -13996,7 +13996,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>45776</v>
@@ -14018,7 +14018,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>45777</v>
@@ -14040,7 +14040,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>45778</v>
@@ -14062,7 +14062,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>45779</v>
@@ -14084,7 +14084,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>45780</v>
@@ -14106,7 +14106,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>45781</v>
@@ -14128,7 +14128,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>45782</v>
@@ -14150,7 +14150,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>45783</v>
@@ -14172,7 +14172,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>45784</v>
@@ -14194,7 +14194,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>45785</v>
@@ -14216,7 +14216,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>45786</v>
@@ -14238,7 +14238,7 @@
         <v>5.21E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>45787</v>
@@ -14260,7 +14260,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>45788</v>
@@ -14282,7 +14282,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>45789</v>
@@ -14304,7 +14304,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>45790</v>
@@ -14326,7 +14326,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>45791</v>
@@ -14348,7 +14348,7 @@
         <v>5.2299999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>45792</v>
@@ -14370,7 +14370,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>45793</v>
@@ -14392,7 +14392,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>45794</v>
@@ -14414,7 +14414,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>45795</v>
@@ -14436,7 +14436,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>45796</v>
@@ -14458,7 +14458,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>45797</v>
@@ -14480,7 +14480,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>45798</v>
@@ -14502,7 +14502,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>45799</v>
@@ -14524,7 +14524,7 @@
         <v>5.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>45800</v>
@@ -14546,7 +14546,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>45801</v>
@@ -14568,7 +14568,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>45802</v>
@@ -14590,7 +14590,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>45803</v>
@@ -14612,7 +14612,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>45804</v>
@@ -14634,7 +14634,7 @@
         <v>5.2699999999999997E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>45805</v>
@@ -14656,7 +14656,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>45806</v>
@@ -14678,7 +14678,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>45807</v>
@@ -14700,7 +14700,7 @@
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>45808</v>
@@ -14722,7 +14722,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>45809</v>
@@ -14744,7 +14744,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>45810</v>
@@ -14766,7 +14766,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>45811</v>
@@ -14788,7 +14788,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>45812</v>
@@ -14810,7 +14810,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>45813</v>
@@ -14832,7 +14832,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>45814</v>
@@ -14854,7 +14854,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>45815</v>
@@ -14876,7 +14876,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>45816</v>
@@ -14898,7 +14898,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>45817</v>
@@ -14920,7 +14920,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>45818</v>
@@ -14942,7 +14942,7 @@
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>45819</v>
@@ -14964,7 +14964,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>45820</v>
@@ -14986,7 +14986,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>45821</v>
@@ -15008,7 +15008,7 @@
         <v>5.0299999999999997E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>45822</v>
@@ -15030,7 +15030,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>45823</v>
@@ -15052,7 +15052,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>45824</v>
@@ -15074,7 +15074,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>45825</v>
@@ -15096,7 +15096,7 @@
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>45826</v>
@@ -15118,7 +15118,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>45827</v>
@@ -15140,7 +15140,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>45828</v>
@@ -15162,7 +15162,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>45829</v>
@@ -15184,7 +15184,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>45830</v>
@@ -15206,7 +15206,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>45831</v>
@@ -15228,7 +15228,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>45832</v>
@@ -15250,7 +15250,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>45833</v>
@@ -15272,7 +15272,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>45834</v>
@@ -15294,7 +15294,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>45835</v>
@@ -15316,7 +15316,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>45836</v>
@@ -15338,7 +15338,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>45837</v>
@@ -15360,7 +15360,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>45838</v>
@@ -15382,7 +15382,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>45839</v>
@@ -15404,7 +15404,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>45840</v>
@@ -15426,7 +15426,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>45841</v>
@@ -15448,7 +15448,7 @@
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>45842</v>
@@ -15470,7 +15470,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>45843</v>
@@ -15492,7 +15492,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>45844</v>
@@ -15514,7 +15514,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>45845</v>
@@ -15536,7 +15536,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>45846</v>
@@ -15558,7 +15558,7 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>45847</v>
@@ -15580,7 +15580,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>45848</v>
@@ -15602,7 +15602,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>45849</v>
@@ -15624,7 +15624,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>45850</v>
@@ -15646,7 +15646,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>45851</v>
@@ -15668,7 +15668,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>45852</v>
@@ -15690,7 +15690,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>45853</v>
@@ -15712,7 +15712,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>45854</v>
@@ -15734,7 +15734,7 @@
         <v>5.11E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>45855</v>
@@ -15756,7 +15756,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>45856</v>
@@ -15778,7 +15778,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>45857</v>
@@ -15800,7 +15800,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>45858</v>
@@ -15822,7 +15822,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>45859</v>
@@ -15844,7 +15844,7 @@
         <v>5.0700000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>45860</v>
@@ -15866,7 +15866,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>45861</v>
@@ -15888,7 +15888,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>45862</v>
@@ -15910,7 +15910,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>45863</v>
@@ -15932,7 +15932,7 @@
         <v>5.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>45864</v>
@@ -15954,7 +15954,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>45865</v>
@@ -15976,7 +15976,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>45866</v>
@@ -15998,7 +15998,7 @@
         <v>4.99E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>45867</v>
@@ -16020,7 +16020,7 @@
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>45868</v>
@@ -16042,7 +16042,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>45869</v>
@@ -16064,7 +16064,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>45870</v>
@@ -16086,7 +16086,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>45871</v>
@@ -16108,7 +16108,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>45872</v>
@@ -16130,7 +16130,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>45873</v>
@@ -16152,7 +16152,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>45874</v>
@@ -16174,7 +16174,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>45875</v>
@@ -16196,7 +16196,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>45876</v>
@@ -16218,7 +16218,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>45877</v>
@@ -16240,7 +16240,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>45878</v>
@@ -16262,7 +16262,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>45879</v>
@@ -16284,7 +16284,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>45880</v>
@@ -16306,7 +16306,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>45881</v>
@@ -16328,7 +16328,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>45882</v>
@@ -16350,7 +16350,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>45883</v>
@@ -16372,7 +16372,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>45884</v>
@@ -16394,7 +16394,7 @@
         <v>4.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>45885</v>
@@ -16416,7 +16416,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>45886</v>
@@ -16438,7 +16438,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>45887</v>
@@ -16460,7 +16460,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>45888</v>
@@ -16482,7 +16482,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>45889</v>
@@ -16504,7 +16504,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>45890</v>
@@ -16526,7 +16526,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>45891</v>
@@ -16548,7 +16548,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>45892</v>
@@ -16570,7 +16570,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>45893</v>
@@ -16592,7 +16592,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>45894</v>
@@ -16614,7 +16614,7 @@
         <v>4.87E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>45895</v>
@@ -16636,7 +16636,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>45896</v>
@@ -16658,7 +16658,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>45897</v>
@@ -16680,7 +16680,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>45898</v>
@@ -16702,7 +16702,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>45899</v>
@@ -16724,7 +16724,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>45900</v>
@@ -16746,7 +16746,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>45901</v>
@@ -16768,7 +16768,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>45902</v>
@@ -16790,7 +16790,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>45903</v>
@@ -16812,7 +16812,7 @@
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>45904</v>
@@ -16834,7 +16834,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>45905</v>
@@ -16856,7 +16856,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>45906</v>
@@ -16878,7 +16878,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>45907</v>
@@ -16900,7 +16900,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>45908</v>
@@ -16922,7 +16922,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>45909</v>
@@ -16944,7 +16944,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>45910</v>
@@ -16966,7 +16966,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>45911</v>
@@ -16988,7 +16988,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>45912</v>
@@ -17010,7 +17010,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>45913</v>
@@ -17032,7 +17032,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>45914</v>
@@ -17054,7 +17054,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>45915</v>
@@ -17076,7 +17076,7 @@
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>45916</v>
@@ -17098,7 +17098,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>45917</v>
@@ -17120,7 +17120,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>45918</v>
@@ -17142,7 +17142,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>45919</v>
@@ -17164,7 +17164,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>45920</v>
@@ -17186,7 +17186,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>45921</v>
@@ -17208,7 +17208,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>45922</v>
@@ -17230,7 +17230,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>45923</v>
@@ -17252,7 +17252,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>45924</v>
@@ -17274,7 +17274,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>45925</v>
@@ -17296,7 +17296,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>45926</v>
@@ -17318,7 +17318,7 @@
         <v>4.7600000000000003E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>45927</v>
@@ -17340,7 +17340,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>45928</v>
@@ -17362,7 +17362,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>45929</v>
@@ -17384,7 +17384,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>45930</v>
@@ -17406,7 +17406,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>45931</v>
@@ -17428,7 +17428,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>45932</v>
@@ -17450,7 +17450,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>45933</v>
@@ -17472,7 +17472,7 @@
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>45934</v>
@@ -17494,7 +17494,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>45935</v>
@@ -17516,7 +17516,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>45936</v>
@@ -17538,7 +17538,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>45937</v>
@@ -17560,7 +17560,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>45938</v>
@@ -17582,7 +17582,7 @@
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>45939</v>
@@ -17604,7 +17604,7 @@
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>45940</v>
@@ -17626,7 +17626,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>45941</v>
@@ -17648,7 +17648,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>45942</v>
@@ -17670,7 +17670,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>45943</v>
@@ -17692,7 +17692,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>45944</v>
@@ -17714,7 +17714,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>45945</v>
@@ -17736,7 +17736,7 @@
         <v>4.65E-2</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>45946</v>
@@ -17758,7 +17758,7 @@
         <v>4.6399999999999997E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>45947</v>
@@ -17780,7 +17780,7 @@
         <v>4.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>45948</v>
@@ -17802,7 +17802,7 @@
         <v>4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>45949</v>
@@ -17824,7 +17824,7 @@
         <v>4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>45950</v>
@@ -17846,7 +17846,7 @@
         <v>4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>45951</v>
@@ -17868,7 +17868,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>45952</v>
@@ -17890,29 +17890,29 @@
         <v>4.58E-2</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>45953</v>
       </c>
-      <c r="B299" s="17" t="str">
+      <c r="B299" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I300</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C299" s="48" t="str">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="C299" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J300</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D299" s="48" t="str">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="D299" s="48">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K300</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E299" s="5" t="str">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="E299" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L300</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.5900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>45954</v>
@@ -17934,7 +17934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>45955</v>
@@ -17956,7 +17956,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>45956</v>
@@ -17978,7 +17978,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>45957</v>
@@ -18000,7 +18000,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>45958</v>
@@ -18022,7 +18022,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>45959</v>
@@ -18044,7 +18044,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>45960</v>
@@ -18066,7 +18066,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>45961</v>
@@ -18088,7 +18088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>45962</v>
@@ -18110,7 +18110,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>45963</v>
@@ -18132,7 +18132,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>45964</v>
@@ -18154,7 +18154,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>45965</v>
@@ -18176,7 +18176,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>45966</v>
@@ -18198,7 +18198,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>45967</v>
@@ -18220,7 +18220,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>45968</v>
@@ -18242,7 +18242,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>45969</v>
@@ -18264,7 +18264,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>45970</v>
@@ -18286,7 +18286,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>45971</v>
@@ -18308,7 +18308,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>45972</v>
@@ -18330,7 +18330,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>45973</v>
@@ -18352,7 +18352,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>45974</v>
@@ -18374,7 +18374,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>45975</v>
@@ -18396,7 +18396,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>45976</v>
@@ -18418,7 +18418,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>45977</v>
@@ -18440,7 +18440,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>45978</v>
@@ -18462,7 +18462,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>45979</v>
@@ -18484,7 +18484,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>45980</v>
@@ -18506,7 +18506,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>45981</v>
@@ -18528,7 +18528,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>45982</v>
@@ -18550,7 +18550,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>45983</v>
@@ -18572,7 +18572,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>45984</v>
@@ -18594,7 +18594,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>45985</v>
@@ -18616,7 +18616,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>45986</v>
@@ -18638,7 +18638,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>45987</v>
@@ -18660,7 +18660,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>45988</v>
@@ -18682,7 +18682,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>45989</v>
@@ -18704,7 +18704,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>45990</v>
@@ -18726,7 +18726,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>45991</v>
@@ -18748,7 +18748,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>45992</v>
@@ -18770,7 +18770,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>45993</v>
@@ -18792,7 +18792,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>45994</v>
@@ -18814,7 +18814,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>45995</v>
@@ -18836,7 +18836,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>45996</v>
@@ -18858,7 +18858,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>45997</v>
@@ -18880,7 +18880,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>45998</v>
@@ -18902,7 +18902,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>45999</v>
@@ -18924,7 +18924,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46000</v>
@@ -18946,7 +18946,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46001</v>
@@ -18968,7 +18968,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46002</v>
@@ -18990,7 +18990,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46003</v>
@@ -19012,7 +19012,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46004</v>
@@ -19034,7 +19034,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46005</v>
@@ -19056,7 +19056,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46006</v>
@@ -19078,7 +19078,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46007</v>
@@ -19100,7 +19100,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46008</v>
@@ -19122,7 +19122,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46009</v>
@@ -19144,7 +19144,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46010</v>
@@ -19166,7 +19166,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46011</v>
@@ -19188,7 +19188,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46012</v>
@@ -19210,7 +19210,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46013</v>
@@ -19232,7 +19232,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46014</v>
@@ -19254,7 +19254,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46015</v>
@@ -19276,7 +19276,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46016</v>
@@ -19298,7 +19298,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46017</v>
@@ -19320,7 +19320,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46018</v>
@@ -19342,7 +19342,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46019</v>
@@ -19364,7 +19364,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46020</v>
@@ -19386,7 +19386,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46021</v>
@@ -19408,7 +19408,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46022</v>
@@ -19430,7 +19430,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="46">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46023</v>
@@ -19452,37 +19452,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -19503,13 +19503,13 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
@@ -19518,14 +19518,14 @@
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="52" t="s">
         <v>5</v>
@@ -19534,7 +19534,7 @@
       <c r="D3" s="53"/>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -19543,7 +19543,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -19560,7 +19560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2025 - 3/31/2025</v>
@@ -19582,7 +19582,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2025 - 6/30/2025</v>
@@ -19604,7 +19604,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2025 - 9/30/2025</v>
@@ -19626,7 +19626,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2025 - 12/31/2025</v>
@@ -19648,7 +19648,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
     </row>
   </sheetData>
@@ -19670,13 +19670,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
@@ -19685,7 +19685,7 @@
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="61" t="s">
         <v>38</v>
       </c>
@@ -19694,12 +19694,12 @@
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="52" t="s">
         <v>10</v>
       </c>
@@ -19708,7 +19708,7 @@
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
@@ -19725,7 +19725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -19749,7 +19749,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -19773,7 +19773,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -19797,7 +19797,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -19821,7 +19821,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -19829,7 +19829,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -19837,7 +19837,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -19847,7 +19847,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>10</v>
       </c>
@@ -19857,7 +19857,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -19897,7 +19897,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -19919,7 +19919,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -19941,7 +19941,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -19963,7 +19963,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -19971,7 +19971,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -19979,7 +19979,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -19989,7 +19989,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>10</v>
       </c>
@@ -19999,7 +19999,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>11</v>
       </c>
@@ -20015,7 +20015,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -20035,7 +20035,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -20055,7 +20055,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -20075,7 +20075,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -20095,7 +20095,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -20104,7 +20104,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -20115,7 +20115,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>10</v>
       </c>
@@ -20126,7 +20126,7 @@
       <c r="F30" s="59"/>
       <c r="G30" s="60"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
@@ -20149,7 +20149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -20184,7 +20184,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>22</v>
       </c>
@@ -20219,7 +20219,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -20254,7 +20254,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -20311,193 +20311,193 @@
       <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="66" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - 22 Table X"</f>
         <v>2025 Q1 VM - 22 Table X</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="64"/>
-      <c r="M1" s="62" t="str" cm="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="M1" s="66" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2025 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
-      <c r="Y1" s="62" t="str" cm="1">
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="68"/>
+      <c r="Y1" s="66" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2025 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AK1" s="62" t="str" cm="1">
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="68"/>
+      <c r="AK1" s="66" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2025 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="64"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="str">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="68"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2024 thru 12/31/2024 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="67"/>
-      <c r="M2" s="65" t="str">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="M2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2025 thru 3/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
-      <c r="Y2" s="65" t="str">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64"/>
+      <c r="Y2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2025 thru 6/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="67"/>
-      <c r="AK2" s="65" t="str">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AK2" s="62" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2025 thru 9/30/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="64"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
       <c r="Y3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="68" t="s">
+      <c r="Z3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="68"/>
-      <c r="AI3" s="68"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="65"/>
       <c r="AK3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AL3" s="68" t="s">
+      <c r="AL3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AM3" s="68"/>
-      <c r="AN3" s="68"/>
-      <c r="AO3" s="68"/>
-      <c r="AP3" s="68"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="68"/>
-      <c r="AU3" s="68"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
@@ -20667,7 +20667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>26</v>
       </c>
@@ -20801,7 +20801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -20975,7 +20975,7 @@
         <v>103.45</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -21149,7 +21149,7 @@
         <v>108.31</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -21323,7 +21323,7 @@
         <v>113.18</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -21497,7 +21497,7 @@
         <v>118.04</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -21671,7 +21671,7 @@
         <v>121.04</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -21845,7 +21845,7 @@
         <v>124.05</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -22019,7 +22019,7 @@
         <v>125.72</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -22193,7 +22193,7 @@
         <v>127.39</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -22367,7 +22367,7 @@
         <v>129.06</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -22541,7 +22541,7 @@
         <v>129.35</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -22715,7 +22715,7 @@
         <v>129.63999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -22889,7 +22889,7 @@
         <v>129.93</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -23063,7 +23063,7 @@
         <v>130.22</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -23237,7 +23237,7 @@
         <v>130.51</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>130.80000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -23585,7 +23585,7 @@
         <v>131.09</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -23759,7 +23759,7 @@
         <v>131.38</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -23933,7 +23933,7 @@
         <v>131.66999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -24107,7 +24107,7 @@
         <v>131.96</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -24281,7 +24281,7 @@
         <v>132.25</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -24455,7 +24455,7 @@
         <v>132.54</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -24629,7 +24629,7 @@
         <v>132.83000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -24803,7 +24803,7 @@
         <v>133.12</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -24977,7 +24977,7 @@
         <v>133.41</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -25151,7 +25151,7 @@
         <v>133.69999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -25325,7 +25325,7 @@
         <v>133.99</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -25499,7 +25499,7 @@
         <v>134.28</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>134.57</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -25847,7 +25847,7 @@
         <v>134.86000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>135.15</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -26197,18 +26197,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26224,7 +26224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection password="9690" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26245,7 +26245,7 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
+                <xdr:colOff>488950</xdr:colOff>
                 <xdr:row>20</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2025-10-31
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2025-vm22-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B4AE04-9B7D-4F09-BADD-C5841C3410DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C8C7DD-AF6D-4421-B38F-FB3061375CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32505" yWindow="2805" windowWidth="21075" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -576,6 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,15 +595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>485775</xdr:colOff>
+          <xdr:colOff>488950</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -9971,17 +9971,17 @@
           <cell r="H307">
             <v>45960</v>
           </cell>
-          <cell r="I307" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J307" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K307" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L307" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I307">
+            <v>3.9100000000000003E-2</v>
+          </cell>
+          <cell r="J307">
+            <v>4.19E-2</v>
+          </cell>
+          <cell r="K307">
+            <v>4.3999999999999997E-2</v>
+          </cell>
+          <cell r="L307">
+            <v>4.6300000000000001E-2</v>
           </cell>
         </row>
         <row r="308">
@@ -11353,19 +11353,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C305" sqref="C305"/>
+      <selection pane="bottomLeft" activeCell="C308" sqref="C308"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="47"/>
       <c r="B1" s="52" t="s">
         <v>4</v>
@@ -11374,7 +11374,7 @@
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -11383,7 +11383,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>45658</v>
@@ -11422,7 +11422,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>45659</v>
@@ -11444,7 +11444,7 @@
         <v>5.0500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>45660</v>
@@ -11466,7 +11466,7 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>45661</v>
@@ -11488,7 +11488,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>45662</v>
@@ -11510,7 +11510,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>45663</v>
@@ -11532,7 +11532,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>45664</v>
@@ -11554,7 +11554,7 @@
         <v>5.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>45665</v>
@@ -11576,7 +11576,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>45666</v>
@@ -11598,7 +11598,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>45667</v>
@@ -11620,7 +11620,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>45668</v>
@@ -11642,7 +11642,7 @@
         <v>5.2400000000000002E-2</v>
       <